<commit_message>
1. add text_io to examine bili module 2. modify bilinear_interpolation_algorithm.txt and bram2vga.xlsx
Signed-off-by: Dvir Hershkovits <dvirhersh@gmail.com>
</commit_message>
<xml_diff>
--- a/datasheets/bram2vga.xlsx
+++ b/datasheets/bram2vga.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital-Zoom-FPGA\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31754023-C3E1-4D2E-B28C-92B915B86AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E14F75-2B64-4DE6-AC78-FC56557584FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9670E6A7-4A90-4DCF-AC2B-294B8B9A454C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>BRAM</t>
   </si>
@@ -72,16 +72,127 @@
   </si>
   <si>
     <t>MONITOR</t>
+  </si>
+  <si>
+    <t>BRAM1</t>
+  </si>
+  <si>
+    <t>BRAM2</t>
+  </si>
+  <si>
+    <t>BILI</t>
+  </si>
+  <si>
+    <t>in:</t>
+  </si>
+  <si>
+    <t>pix1</t>
+  </si>
+  <si>
+    <t>pix2</t>
+  </si>
+  <si>
+    <t>pix3</t>
+  </si>
+  <si>
+    <t>pix4</t>
+  </si>
+  <si>
+    <t>out:</t>
+  </si>
+  <si>
+    <t>pix16</t>
+  </si>
+  <si>
+    <t>pix5</t>
+  </si>
+  <si>
+    <t>pix9</t>
+  </si>
+  <si>
+    <t>pix15</t>
+  </si>
+  <si>
+    <t>pix6</t>
+  </si>
+  <si>
+    <t>pix7</t>
+  </si>
+  <si>
+    <t>pix8</t>
+  </si>
+  <si>
+    <t>pix10</t>
+  </si>
+  <si>
+    <t>pix11</t>
+  </si>
+  <si>
+    <t>pix12</t>
+  </si>
+  <si>
+    <t>pix13</t>
+  </si>
+  <si>
+    <t>pix14</t>
+  </si>
+  <si>
+    <t>read:</t>
+  </si>
+  <si>
+    <t>dina</t>
+  </si>
+  <si>
+    <t>wea</t>
+  </si>
+  <si>
+    <t>write:</t>
+  </si>
+  <si>
+    <t>addra</t>
+  </si>
+  <si>
+    <t>addrb</t>
+  </si>
+  <si>
+    <t>doutb</t>
+  </si>
+  <si>
+    <t>clka - 25MHz</t>
+  </si>
+  <si>
+    <t>clkb - 25MHz</t>
+  </si>
+  <si>
+    <t>clk_bili - 6.25MHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pix1 - 0 </t>
+  </si>
+  <si>
+    <t>pix2 - 1</t>
+  </si>
+  <si>
+    <t>pix3 - 320</t>
+  </si>
+  <si>
+    <t>pix4 - 321</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -223,9 +334,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -233,35 +343,31 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,529 +702,719 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05C238A-0561-4BB7-9A92-291FE0D71310}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:V41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="G2" s="6">
         <v>1</v>
       </c>
-      <c r="D2" s="3">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="31">
+        <v>319</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="5">
+        <v>0</v>
+      </c>
+      <c r="S2" s="27">
+        <v>0.3</v>
+      </c>
+      <c r="T2" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="U2" s="16">
         <v>1</v>
       </c>
-      <c r="F2" s="6">
+      <c r="V2" s="28"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="G2" s="7">
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="16">
         <v>1</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="9">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8">
+        <v>320</v>
+      </c>
+      <c r="G3" s="4">
+        <v>321</v>
+      </c>
+      <c r="J3" s="32">
+        <v>639</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="10"/>
+      <c r="Q3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="25">
+        <v>106.6</v>
+      </c>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="26">
+        <v>101</v>
+      </c>
+      <c r="V3" s="26"/>
+    </row>
+    <row r="4" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>320</v>
+      </c>
+      <c r="B4" s="17">
+        <v>320</v>
+      </c>
+      <c r="C4" s="18">
+        <v>321</v>
+      </c>
+      <c r="D4" s="4">
+        <v>321</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="J4" s="30"/>
+      <c r="L4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" s="9">
+        <v>210</v>
+      </c>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="10">
+        <v>202</v>
+      </c>
+      <c r="V4" s="10"/>
+    </row>
+    <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>320</v>
+      </c>
+      <c r="B5" s="3">
+        <v>320</v>
+      </c>
+      <c r="C5" s="4">
+        <v>321</v>
+      </c>
+      <c r="D5" s="4">
+        <v>321</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="J5" s="30"/>
+      <c r="L5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" s="17">
+        <v>320</v>
+      </c>
+      <c r="S5" s="12">
+        <v>320.3</v>
+      </c>
+      <c r="T5" s="12">
+        <v>320.60000000000002</v>
+      </c>
+      <c r="U5" s="18">
+        <v>321</v>
+      </c>
+      <c r="V5" s="10"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F6" s="9"/>
+      <c r="J6" s="30"/>
+      <c r="L6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6" s="9"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="10"/>
+    </row>
+    <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="9"/>
+      <c r="J7" s="30"/>
+      <c r="L7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>36</v>
+      </c>
+      <c r="R7" s="9"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="30"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="10"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="5">
         <v>0</v>
       </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="25">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="16">
         <v>1</v>
       </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="10">
+      <c r="F8" s="9"/>
+      <c r="J8" s="30"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>38</v>
+      </c>
+      <c r="R8" s="9"/>
+      <c r="S8" s="30"/>
+      <c r="T8" s="30"/>
+      <c r="U8" s="30"/>
+      <c r="V8" s="10"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="9"/>
+      <c r="J9" s="30"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>41</v>
+      </c>
+      <c r="R9" s="9"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="30"/>
+      <c r="V9" s="10"/>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11">
+        <v>76480</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12">
+        <v>76799</v>
+      </c>
+      <c r="L10" s="9"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10" s="11">
+        <v>76480</v>
+      </c>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="13">
+        <v>76799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="17">
         <v>320</v>
       </c>
-      <c r="G3" s="11">
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="18">
         <v>321</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="13">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>320</v>
-      </c>
-      <c r="B4" s="26">
-        <v>320</v>
-      </c>
-      <c r="C4" s="27">
-        <v>321</v>
-      </c>
-      <c r="D4" s="5">
-        <v>321</v>
-      </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="16"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>320</v>
-      </c>
-      <c r="B5" s="4">
-        <v>320</v>
-      </c>
-      <c r="C5" s="5">
-        <v>321</v>
-      </c>
-      <c r="D5" s="5">
-        <v>321</v>
-      </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="16"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="16"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="16"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="25">
-        <v>1</v>
-      </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="16"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="16"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="23"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17">
-        <v>76480</v>
-      </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="20">
-        <v>76799</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="26">
-        <v>320</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="27">
-        <v>321</v>
-      </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="22"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F12" s="23"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F13" s="23"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F11" s="14"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="R11" s="14"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="15"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F12" s="9"/>
+      <c r="J12" s="30"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="R12" s="9"/>
+      <c r="V12" s="10"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F13" s="9"/>
+      <c r="J13" s="30"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="R13" s="9"/>
+      <c r="V13" s="10"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="16"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F14" s="9"/>
+      <c r="J14" s="30"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="R14" s="9"/>
+      <c r="V14" s="10"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="16"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F15" s="9"/>
+      <c r="J15" s="30"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="R15" s="9"/>
+      <c r="V15" s="10"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="16"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F16" s="9"/>
+      <c r="J16" s="30"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="R16" s="9"/>
+      <c r="V16" s="10"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="23"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="16"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F17" s="9"/>
+      <c r="J17" s="30"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R17" s="9"/>
+      <c r="V17" s="10"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="23"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="16"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F18" s="9"/>
+      <c r="J18" s="30"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="R18" s="9"/>
+      <c r="V18" s="10"/>
+    </row>
+    <row r="19" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>5</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="23"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="16"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F20" s="23"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="16"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F21" s="23"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="16"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F22" s="23"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="16"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F23" s="23"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="16"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F24" s="23"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="16"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F25" s="23"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="16"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F26" s="23"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="16"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F27" s="23"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="16"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F28" s="23"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="16"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F29" s="23"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="16"/>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F30" s="24"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="20">
+      <c r="F19" s="9"/>
+      <c r="J19" s="30"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="R19" s="9"/>
+      <c r="V19" s="10"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F20" s="9"/>
+      <c r="J20" s="10"/>
+      <c r="R20" s="9"/>
+      <c r="V20" s="10"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F21" s="9"/>
+      <c r="J21" s="10"/>
+      <c r="R21" s="9"/>
+      <c r="V21" s="10"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F22" s="9"/>
+      <c r="J22" s="10"/>
+      <c r="R22" s="9"/>
+      <c r="V22" s="10"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F23" s="9"/>
+      <c r="J23" s="10"/>
+      <c r="R23" s="9"/>
+      <c r="V23" s="10"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F24" s="9"/>
+      <c r="J24" s="10"/>
+      <c r="R24" s="9"/>
+      <c r="V24" s="10"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F25" s="9"/>
+      <c r="J25" s="10"/>
+      <c r="R25" s="9"/>
+      <c r="V25" s="10"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F26" s="9"/>
+      <c r="J26" s="10"/>
+      <c r="R26" s="9"/>
+      <c r="V26" s="10"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F27" s="9"/>
+      <c r="J27" s="10"/>
+      <c r="R27" s="9"/>
+      <c r="V27" s="10"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F28" s="9"/>
+      <c r="J28" s="10"/>
+      <c r="R28" s="9"/>
+      <c r="V28" s="10"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F29" s="9"/>
+      <c r="J29" s="10"/>
+      <c r="R29" s="9"/>
+      <c r="V29" s="10"/>
+    </row>
+    <row r="30" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="11"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="13">
+        <v>307199</v>
+      </c>
+      <c r="R30" s="11"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="13">
         <v>307199</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="22"/>
-      <c r="G34" s="21" t="s">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="15"/>
+      <c r="G34" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="22"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="15"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
+      <c r="A35" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="5">
         <v>10</v>
       </c>
-      <c r="C35" s="25">
+      <c r="C35" s="16">
         <v>20</v>
       </c>
-      <c r="D35" s="12"/>
-      <c r="E35" s="16"/>
-      <c r="G35" s="6">
+      <c r="E35" s="10"/>
+      <c r="G35" s="5">
         <v>10</v>
       </c>
-      <c r="H35" s="25">
+      <c r="H35" s="16">
         <v>20</v>
       </c>
-      <c r="I35" s="12"/>
-      <c r="J35" s="16"/>
+      <c r="J35" s="10"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="23"/>
-      <c r="B36" s="26">
+      <c r="A36" s="9"/>
+      <c r="B36" s="17">
         <v>30</v>
       </c>
-      <c r="C36" s="27">
+      <c r="C36" s="18">
         <v>40</v>
       </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="16"/>
-      <c r="G36" s="26">
+      <c r="E36" s="10"/>
+      <c r="G36" s="17">
         <v>30</v>
       </c>
-      <c r="H36" s="27">
+      <c r="H36" s="18">
         <v>40</v>
       </c>
-      <c r="I36" s="12"/>
-      <c r="J36" s="16"/>
+      <c r="J36" s="10"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="23"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="16"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="16"/>
+      <c r="A37" s="9"/>
+      <c r="E37" s="10"/>
+      <c r="G37" s="9"/>
+      <c r="J37" s="10"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="5">
         <v>10</v>
       </c>
-      <c r="C38" s="32">
+      <c r="C38" s="19">
         <v>10</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="6">
         <v>20</v>
       </c>
-      <c r="E38" s="25">
+      <c r="E38" s="16">
         <v>20</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38" s="5">
         <v>10</v>
       </c>
-      <c r="H38" s="12">
+      <c r="H38">
         <v>13</v>
       </c>
-      <c r="I38" s="12">
+      <c r="I38">
         <v>16</v>
       </c>
-      <c r="J38" s="25">
+      <c r="J38" s="16">
         <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
-      <c r="B39" s="33">
+      <c r="A39" s="9"/>
+      <c r="B39" s="20">
         <v>10</v>
       </c>
-      <c r="C39" s="29">
+      <c r="C39" s="1">
         <v>10</v>
       </c>
-      <c r="D39" s="30">
+      <c r="D39" s="2">
         <v>20</v>
       </c>
-      <c r="E39" s="34">
+      <c r="E39" s="21">
         <v>20</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="9">
         <v>15</v>
       </c>
-      <c r="H39" s="15">
+      <c r="H39">
         <v>18</v>
       </c>
-      <c r="I39" s="15">
+      <c r="I39">
         <v>21</v>
       </c>
-      <c r="J39" s="28">
+      <c r="J39" s="10">
         <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="10">
+      <c r="A40" s="9"/>
+      <c r="B40" s="8">
         <v>30</v>
       </c>
-      <c r="C40" s="31">
+      <c r="C40" s="3">
         <v>30</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D40" s="4">
         <v>40</v>
       </c>
-      <c r="E40" s="35">
+      <c r="E40" s="22">
         <v>40</v>
       </c>
-      <c r="G40" s="23">
+      <c r="G40" s="9">
         <v>25</v>
       </c>
-      <c r="H40" s="15">
+      <c r="H40">
         <v>28</v>
       </c>
-      <c r="I40" s="12">
+      <c r="I40">
         <v>31</v>
       </c>
-      <c r="J40" s="16">
+      <c r="J40" s="10">
         <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="24"/>
-      <c r="B41" s="26">
+      <c r="A41" s="11"/>
+      <c r="B41" s="17">
         <v>30</v>
       </c>
-      <c r="C41" s="36">
+      <c r="C41" s="23">
         <v>30</v>
       </c>
-      <c r="D41" s="37">
+      <c r="D41" s="24">
         <v>40</v>
       </c>
-      <c r="E41" s="27">
+      <c r="E41" s="18">
         <v>40</v>
       </c>
-      <c r="G41" s="26">
+      <c r="G41" s="17">
         <v>30</v>
       </c>
-      <c r="H41" s="19">
+      <c r="H41" s="12">
         <v>33</v>
       </c>
-      <c r="I41" s="19">
+      <c r="I41" s="12">
         <v>36</v>
       </c>
-      <c r="J41" s="27">
+      <c r="J41" s="18">
         <v>40</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
bram2vga.xlsx - add big bili
Signed-off-by: Dvir Hershkovits <dvirhersh@gmail.com>
</commit_message>
<xml_diff>
--- a/datasheets/bram2vga.xlsx
+++ b/datasheets/bram2vga.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital-Zoom-FPGA\datasheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3f0ace79a29258c/שולחן העבודה/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E14F75-2B64-4DE6-AC78-FC56557584FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{188B935E-08FF-4423-8627-4C91C6A50C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F73A572-31FA-4D60-8FA9-B1F0355E99C0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9670E6A7-4A90-4DCF-AC2B-294B8B9A454C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>BRAM</t>
   </si>
@@ -47,24 +47,6 @@
     <t>in vga.vhd</t>
   </si>
   <si>
-    <t>tasks:</t>
-  </si>
-  <si>
-    <t>remove duplication mechnism from vga.vhd</t>
-  </si>
-  <si>
-    <t>create duplicator module between BRAM and vga.vhd</t>
-  </si>
-  <si>
-    <t>verify that everything works as usuall</t>
-  </si>
-  <si>
-    <t>create bili module after the duplicator</t>
-  </si>
-  <si>
-    <t>another BRAM</t>
-  </si>
-  <si>
     <t>current simulation:</t>
   </si>
   <si>
@@ -80,9 +62,6 @@
     <t>BRAM2</t>
   </si>
   <si>
-    <t>BILI</t>
-  </si>
-  <si>
     <t>in:</t>
   </si>
   <si>
@@ -164,9 +143,6 @@
     <t>clkb - 25MHz</t>
   </si>
   <si>
-    <t>clk_bili - 6.25MHz</t>
-  </si>
-  <si>
     <t xml:space="preserve">pix1 - 0 </t>
   </si>
   <si>
@@ -177,6 +153,25 @@
   </si>
   <si>
     <t>pix4 - 321</t>
+  </si>
+  <si>
+    <t>clk_bili - 6.25MHz
+or 25MHz</t>
+  </si>
+  <si>
+    <t>BILI_big</t>
+  </si>
+  <si>
+    <t>BILI_small</t>
+  </si>
+  <si>
+    <t>clk_bili_small
+6.25MHz
+(160nS)</t>
+  </si>
+  <si>
+    <t>16 pixels
+(after time calc)</t>
   </si>
 </sst>
 </file>
@@ -334,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -343,7 +338,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -366,8 +363,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,14 +709,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05C238A-0561-4BB7-9A92-291FE0D71310}">
   <dimension ref="A1:V41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:V30"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -722,16 +730,16 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="M1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="R1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -752,110 +760,115 @@
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="31">
+      <c r="J2" s="8">
         <v>319</v>
       </c>
-      <c r="L2" s="14" t="s">
-        <v>15</v>
+      <c r="L2" s="16" t="s">
+        <v>8</v>
       </c>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
-      <c r="O2" s="15" t="s">
-        <v>20</v>
+      <c r="O2" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="Q2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="R2" s="5">
         <v>0</v>
       </c>
-      <c r="S2" s="27">
-        <v>0.3</v>
-      </c>
-      <c r="T2" s="27">
+      <c r="S2" s="29"/>
+      <c r="T2" s="29">
         <v>0.6</v>
       </c>
-      <c r="U2" s="16">
+      <c r="U2" s="18">
         <v>1</v>
       </c>
-      <c r="V2" s="28"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V2" s="30"/>
+    </row>
+    <row r="3" spans="1:22" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="36">
         <v>0</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="37">
         <v>1</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="9">
         <v>320</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="33">
         <v>321</v>
       </c>
-      <c r="J3" s="32">
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="10">
         <v>639</v>
       </c>
-      <c r="L3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="10"/>
+      <c r="L3" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="12"/>
       <c r="Q3" t="s">
-        <v>37</v>
-      </c>
-      <c r="R3" s="25">
+        <v>30</v>
+      </c>
+      <c r="R3" s="27">
         <v>106.6</v>
       </c>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="26">
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="28">
         <v>101</v>
       </c>
-      <c r="V3" s="26"/>
-    </row>
-    <row r="4" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V3" s="28"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>320</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="38">
         <v>320</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="33">
         <v>321</v>
       </c>
       <c r="D4" s="4">
         <v>321</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="J4" s="30"/>
-      <c r="L4" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="10" t="s">
-        <v>16</v>
+      <c r="F4" s="11"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="12"/>
+      <c r="L4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="17"/>
+      <c r="O4" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="Q4" t="s">
-        <v>40</v>
-      </c>
-      <c r="R4" s="9">
+        <v>33</v>
+      </c>
+      <c r="R4" s="11">
         <v>210</v>
       </c>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="10">
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="12">
         <v>202</v>
       </c>
-      <c r="V4" s="10"/>
+      <c r="V4" s="12"/>
     </row>
     <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
@@ -870,453 +883,493 @@
       <c r="D5" s="4">
         <v>321</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="J5" s="30"/>
-      <c r="L5" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="10" t="s">
-        <v>17</v>
+      <c r="F5" s="11"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="12"/>
+      <c r="L5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="Q5" t="s">
+        <v>27</v>
+      </c>
+      <c r="R5" s="19">
+        <v>320</v>
+      </c>
+      <c r="S5" s="14">
+        <v>320.3</v>
+      </c>
+      <c r="T5" s="14">
+        <v>320.60000000000002</v>
+      </c>
+      <c r="U5" s="20">
+        <v>321</v>
+      </c>
+      <c r="V5" s="12"/>
+    </row>
+    <row r="6" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="F6" s="11"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="12"/>
+      <c r="L6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" s="11"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="32"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="12"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F7" s="11"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="12"/>
+      <c r="L7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="11"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" s="11"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="32"/>
+      <c r="V7" s="12"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="12"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R8" s="11"/>
+      <c r="S8" s="32"/>
+      <c r="T8" s="32"/>
+      <c r="U8" s="32"/>
+      <c r="V8" s="12"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="12"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9" t="s">
         <v>34</v>
       </c>
-      <c r="R5" s="17">
-        <v>320</v>
-      </c>
-      <c r="S5" s="12">
-        <v>320.3</v>
-      </c>
-      <c r="T5" s="12">
-        <v>320.60000000000002</v>
-      </c>
-      <c r="U5" s="18">
-        <v>321</v>
-      </c>
-      <c r="V5" s="10"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F6" s="9"/>
-      <c r="J6" s="30"/>
-      <c r="L6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R6" s="9"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="10"/>
-    </row>
-    <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F7" s="9"/>
-      <c r="J7" s="30"/>
-      <c r="L7" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="10" t="s">
+      <c r="R9" s="11"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="12"/>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="13">
+        <v>76480</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="15">
+        <v>76799</v>
+      </c>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" t="s">
-        <v>36</v>
-      </c>
-      <c r="R7" s="9"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="10"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
-        <v>0</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="16">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="J8" s="30"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>38</v>
-      </c>
-      <c r="R8" s="9"/>
-      <c r="S8" s="30"/>
-      <c r="T8" s="30"/>
-      <c r="U8" s="30"/>
-      <c r="V8" s="10"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="9"/>
-      <c r="J9" s="30"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>41</v>
-      </c>
-      <c r="R9" s="9"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="10"/>
-    </row>
-    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="9"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11">
+      <c r="Q10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R10" s="13">
         <v>76480</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12">
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="15">
         <v>76799</v>
       </c>
-      <c r="L10" s="9"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>39</v>
-      </c>
-      <c r="R10" s="11">
-        <v>76480</v>
-      </c>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="13">
-        <v>76799</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="17">
-        <v>320</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="18">
-        <v>321</v>
-      </c>
-      <c r="F11" s="14"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="16"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="R11" s="14"/>
+      <c r="J11" s="17"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="R11" s="16"/>
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
       <c r="U11" s="7"/>
-      <c r="V11" s="15"/>
+      <c r="V11" s="17"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F12" s="9"/>
-      <c r="J12" s="30"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="10" t="s">
+      <c r="F12" s="11"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="12"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="R12" s="11"/>
+      <c r="V12" s="12"/>
+    </row>
+    <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="11"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="12"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="R13" s="11"/>
+      <c r="V13" s="12"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F14" s="11"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="12"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="R14" s="11"/>
+      <c r="V14" s="12"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F15" s="11"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="12"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="R12" s="9"/>
-      <c r="V12" s="10"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F13" s="9"/>
-      <c r="J13" s="30"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="R13" s="9"/>
-      <c r="V13" s="10"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="J14" s="30"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="R14" s="9"/>
-      <c r="V14" s="10"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="J15" s="30"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="R15" s="9"/>
-      <c r="V15" s="10"/>
+      <c r="R15" s="11"/>
+      <c r="V15" s="12"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="9"/>
-      <c r="J16" s="30"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="R16" s="9"/>
-      <c r="V16" s="10"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="J17" s="30"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="R17" s="9"/>
-      <c r="V17" s="10"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="9"/>
-      <c r="J18" s="30"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="10" t="s">
+      <c r="F16" s="11"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="12"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R18" s="9"/>
-      <c r="V18" s="10"/>
-    </row>
-    <row r="19" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="9"/>
-      <c r="J19" s="30"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="R19" s="9"/>
-      <c r="V19" s="10"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F20" s="9"/>
-      <c r="J20" s="10"/>
-      <c r="R20" s="9"/>
-      <c r="V20" s="10"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F21" s="9"/>
-      <c r="J21" s="10"/>
-      <c r="R21" s="9"/>
-      <c r="V21" s="10"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F22" s="9"/>
-      <c r="J22" s="10"/>
-      <c r="R22" s="9"/>
-      <c r="V22" s="10"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F23" s="9"/>
-      <c r="J23" s="10"/>
-      <c r="R23" s="9"/>
-      <c r="V23" s="10"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F24" s="9"/>
-      <c r="J24" s="10"/>
-      <c r="R24" s="9"/>
-      <c r="V24" s="10"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F25" s="9"/>
-      <c r="J25" s="10"/>
-      <c r="R25" s="9"/>
-      <c r="V25" s="10"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F26" s="9"/>
-      <c r="J26" s="10"/>
-      <c r="R26" s="9"/>
-      <c r="V26" s="10"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F27" s="9"/>
-      <c r="J27" s="10"/>
-      <c r="R27" s="9"/>
-      <c r="V27" s="10"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F28" s="9"/>
-      <c r="J28" s="10"/>
-      <c r="R28" s="9"/>
-      <c r="V28" s="10"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F29" s="9"/>
-      <c r="J29" s="10"/>
-      <c r="R29" s="9"/>
-      <c r="V29" s="10"/>
-    </row>
-    <row r="30" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F30" s="11"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="13">
+      <c r="R16" s="11"/>
+      <c r="V16" s="12"/>
+    </row>
+    <row r="17" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F17" s="11"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="12"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="R17" s="11"/>
+      <c r="V17" s="12"/>
+    </row>
+    <row r="18" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F18" s="11"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="12"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="R18" s="11"/>
+      <c r="V18" s="12"/>
+    </row>
+    <row r="19" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="11"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="12"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="R19" s="11"/>
+      <c r="V19" s="12"/>
+    </row>
+    <row r="20" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F20" s="11"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="12"/>
+      <c r="R20" s="11"/>
+      <c r="V20" s="12"/>
+    </row>
+    <row r="21" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F21" s="11"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="12"/>
+      <c r="R21" s="11"/>
+      <c r="V21" s="12"/>
+    </row>
+    <row r="22" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F22" s="11"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="12"/>
+      <c r="R22" s="11"/>
+      <c r="V22" s="12"/>
+    </row>
+    <row r="23" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F23" s="11"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="12"/>
+      <c r="R23" s="11"/>
+      <c r="V23" s="12"/>
+    </row>
+    <row r="24" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F24" s="11"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="12"/>
+      <c r="R24" s="11"/>
+      <c r="V24" s="12"/>
+    </row>
+    <row r="25" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F25" s="11"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="12"/>
+      <c r="R25" s="11"/>
+      <c r="V25" s="12"/>
+    </row>
+    <row r="26" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F26" s="11"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="12"/>
+      <c r="R26" s="11"/>
+      <c r="V26" s="12"/>
+    </row>
+    <row r="27" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F27" s="11"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="12"/>
+      <c r="R27" s="11"/>
+      <c r="V27" s="12"/>
+    </row>
+    <row r="28" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F28" s="11"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="12"/>
+      <c r="R28" s="11"/>
+      <c r="V28" s="12"/>
+    </row>
+    <row r="29" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F29" s="11"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="12"/>
+      <c r="R29" s="11"/>
+      <c r="V29" s="12"/>
+    </row>
+    <row r="30" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="15">
         <v>307199</v>
       </c>
-      <c r="R30" s="11"/>
-      <c r="S30" s="12"/>
-      <c r="T30" s="12"/>
-      <c r="U30" s="12"/>
-      <c r="V30" s="13">
+      <c r="R30" s="13"/>
+      <c r="S30" s="14"/>
+      <c r="T30" s="14"/>
+      <c r="U30" s="14"/>
+      <c r="V30" s="15">
         <v>307199</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
-        <v>9</v>
+      <c r="A34" s="16" t="s">
+        <v>3</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
-      <c r="E34" s="15"/>
-      <c r="G34" s="14" t="s">
-        <v>10</v>
+      <c r="E34" s="17"/>
+      <c r="G34" s="16" t="s">
+        <v>4</v>
       </c>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
-      <c r="J34" s="15"/>
+      <c r="J34" s="17"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B35" s="5">
         <v>10</v>
       </c>
-      <c r="C35" s="16">
+      <c r="C35" s="18">
         <v>20</v>
       </c>
-      <c r="E35" s="10"/>
+      <c r="E35" s="12"/>
       <c r="G35" s="5">
         <v>10</v>
       </c>
-      <c r="H35" s="16">
+      <c r="H35" s="18">
         <v>20</v>
       </c>
-      <c r="J35" s="10"/>
+      <c r="J35" s="12"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="9"/>
-      <c r="B36" s="17">
+      <c r="A36" s="11"/>
+      <c r="B36" s="19">
         <v>30</v>
       </c>
-      <c r="C36" s="18">
+      <c r="C36" s="20">
         <v>40</v>
       </c>
-      <c r="E36" s="10"/>
-      <c r="G36" s="17">
+      <c r="E36" s="12"/>
+      <c r="G36" s="19">
         <v>30</v>
       </c>
-      <c r="H36" s="18">
+      <c r="H36" s="20">
         <v>40</v>
       </c>
-      <c r="J36" s="10"/>
+      <c r="J36" s="12"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="9"/>
-      <c r="E37" s="10"/>
-      <c r="G37" s="9"/>
-      <c r="J37" s="10"/>
+      <c r="A37" s="11"/>
+      <c r="E37" s="12"/>
+      <c r="G37" s="11"/>
+      <c r="J37" s="12"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>11</v>
+      <c r="A38" s="11" t="s">
+        <v>5</v>
       </c>
       <c r="B38" s="5">
         <v>10</v>
       </c>
-      <c r="C38" s="19">
+      <c r="C38" s="21">
         <v>10</v>
       </c>
       <c r="D38" s="6">
         <v>20</v>
       </c>
-      <c r="E38" s="16">
+      <c r="E38" s="18">
         <v>20</v>
       </c>
       <c r="G38" s="5">
@@ -1328,13 +1381,13 @@
       <c r="I38">
         <v>16</v>
       </c>
-      <c r="J38" s="16">
+      <c r="J38" s="18">
         <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
-      <c r="B39" s="20">
+      <c r="A39" s="11"/>
+      <c r="B39" s="22">
         <v>10</v>
       </c>
       <c r="C39" s="1">
@@ -1343,10 +1396,10 @@
       <c r="D39" s="2">
         <v>20</v>
       </c>
-      <c r="E39" s="21">
+      <c r="E39" s="23">
         <v>20</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="11">
         <v>15</v>
       </c>
       <c r="H39">
@@ -1355,13 +1408,13 @@
       <c r="I39">
         <v>21</v>
       </c>
-      <c r="J39" s="10">
+      <c r="J39" s="12">
         <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="8">
+      <c r="A40" s="11"/>
+      <c r="B40" s="9">
         <v>30</v>
       </c>
       <c r="C40" s="3">
@@ -1370,10 +1423,10 @@
       <c r="D40" s="4">
         <v>40</v>
       </c>
-      <c r="E40" s="22">
+      <c r="E40" s="24">
         <v>40</v>
       </c>
-      <c r="G40" s="9">
+      <c r="G40" s="11">
         <v>25</v>
       </c>
       <c r="H40">
@@ -1382,34 +1435,34 @@
       <c r="I40">
         <v>31</v>
       </c>
-      <c r="J40" s="10">
+      <c r="J40" s="12">
         <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="11"/>
-      <c r="B41" s="17">
+      <c r="A41" s="13"/>
+      <c r="B41" s="19">
         <v>30</v>
       </c>
-      <c r="C41" s="23">
+      <c r="C41" s="25">
         <v>30</v>
       </c>
-      <c r="D41" s="24">
+      <c r="D41" s="26">
         <v>40</v>
       </c>
-      <c r="E41" s="18">
+      <c r="E41" s="20">
         <v>40</v>
       </c>
-      <c r="G41" s="17">
+      <c r="G41" s="19">
         <v>30</v>
       </c>
-      <c r="H41" s="12">
+      <c r="H41" s="14">
         <v>33</v>
       </c>
-      <c r="I41" s="12">
+      <c r="I41" s="14">
         <v>36</v>
       </c>
-      <c r="J41" s="18">
+      <c r="J41" s="20">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refining bili algorithm in the xlx file .
Signed-off-by: idowein <ido.weinstock@gmail.com>
</commit_message>
<xml_diff>
--- a/datasheets/bram2vga.xlsx
+++ b/datasheets/bram2vga.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3f0ace79a29258c/שולחן העבודה/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idowe\Projects\Digital-Zoom-FPGA\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{188B935E-08FF-4423-8627-4C91C6A50C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F73A572-31FA-4D60-8FA9-B1F0355E99C0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B1431C-55A4-4C3B-B63E-0D2F81C44A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9670E6A7-4A90-4DCF-AC2B-294B8B9A454C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="67">
   <si>
     <t>BRAM</t>
   </si>
@@ -137,26 +137,10 @@
     <t>doutb</t>
   </si>
   <si>
-    <t>clka - 25MHz</t>
-  </si>
-  <si>
     <t>clkb - 25MHz</t>
   </si>
   <si>
     <t xml:space="preserve">pix1 - 0 </t>
-  </si>
-  <si>
-    <t>pix2 - 1</t>
-  </si>
-  <si>
-    <t>pix3 - 320</t>
-  </si>
-  <si>
-    <t>pix4 - 321</t>
-  </si>
-  <si>
-    <t>clk_bili - 6.25MHz
-or 25MHz</t>
   </si>
   <si>
     <t>BILI_big</t>
@@ -172,28 +156,142 @@
   <si>
     <t>16 pixels
 (after time calc)</t>
+  </si>
+  <si>
+    <t>clka - 25 mhz</t>
+  </si>
+  <si>
+    <t>clkb - 25 mhz</t>
+  </si>
+  <si>
+    <t>clk_bili_big_ 25 mhz</t>
+  </si>
+  <si>
+    <t>pix2 - 40 ns</t>
+  </si>
+  <si>
+    <t>pix3 - 80</t>
+  </si>
+  <si>
+    <t>pix4 - 120</t>
+  </si>
+  <si>
+    <t>clk_bili_small 5mhz</t>
+  </si>
+  <si>
+    <t>Example:</t>
+  </si>
+  <si>
+    <t>4 pixels - 120 ns</t>
+  </si>
+  <si>
+    <t>Round 1</t>
+  </si>
+  <si>
+    <t>output - 360 ns (After one 5mhz clock)</t>
+  </si>
+  <si>
+    <t>5 mhz</t>
+  </si>
+  <si>
+    <t>( 200 ns / 16 px ) = 12.5 ns -&gt; 80 mhz</t>
+  </si>
+  <si>
+    <t>clka - 80MHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pix 4 - 280 </t>
+  </si>
+  <si>
+    <t>output to small bili - 320</t>
+  </si>
+  <si>
+    <t>pix 6 &amp; output x 4 - 200</t>
+  </si>
+  <si>
+    <t>pix 5 &amp; output x 4 - 160</t>
+  </si>
+  <si>
+    <t>pix 7 &amp; output x 4 - 240</t>
+  </si>
+  <si>
+    <t>pix 7  - 240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clk_bili_small
+</t>
+  </si>
+  <si>
+    <t>clk_bili_small 6.25mhz</t>
+  </si>
+  <si>
+    <t>100 mhz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pix 8 - 280 </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">pix 5 &amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>output x 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - 160</t>
+    </r>
+  </si>
+  <si>
+    <t>לחשב בלי אנסיינגד אלא עם דאון-טו</t>
+  </si>
+  <si>
+    <t>להתחי להרכיב את העסק</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,6 +331,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -357,22 +467,23 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,20 +820,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05C238A-0561-4BB7-9A92-291FE0D71310}">
   <dimension ref="A1:V41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G3"/>
+    <sheetView tabSelected="1" topLeftCell="L17" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12.875" customWidth="1"/>
+    <col min="12" max="13" width="23.25" customWidth="1"/>
+    <col min="16" max="16" width="30.375" customWidth="1"/>
+    <col min="17" max="17" width="11.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -733,13 +843,13 @@
         <v>6</v>
       </c>
       <c r="M1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="R1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -777,23 +887,23 @@
       <c r="R2" s="5">
         <v>0</v>
       </c>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29">
+      <c r="S2" s="7"/>
+      <c r="T2" s="7">
         <v>0.6</v>
       </c>
       <c r="U2" s="18">
         <v>1</v>
       </c>
-      <c r="V2" s="30"/>
-    </row>
-    <row r="3" spans="1:22" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V2" s="17"/>
+    </row>
+    <row r="3" spans="1:22" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2">
@@ -802,75 +912,70 @@
       <c r="F3" s="9">
         <v>320</v>
       </c>
-      <c r="G3" s="33">
+      <c r="G3" s="4">
         <v>321</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
       <c r="J3" s="10">
         <v>639</v>
       </c>
-      <c r="L3" s="34" t="s">
+      <c r="K3" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
+      <c r="L3" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
       <c r="O3" s="12"/>
       <c r="Q3" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="27">
+      <c r="R3" s="11">
         <v>106.6</v>
       </c>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="28">
+      <c r="U3" s="12">
         <v>101</v>
       </c>
-      <c r="V3" s="28"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V3" s="12"/>
+    </row>
+    <row r="4" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>320</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="3">
         <v>320</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C4" s="4">
         <v>321</v>
       </c>
       <c r="D4" s="4">
         <v>321</v>
       </c>
       <c r="F4" s="11"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
       <c r="J4" s="12"/>
-      <c r="L4" s="11" t="s">
-        <v>35</v>
-      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="11"/>
       <c r="M4" s="16" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="N4" s="17"/>
       <c r="O4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="Q4" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="R4" s="11">
         <v>210</v>
       </c>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
       <c r="U4" s="12">
         <v>202</v>
       </c>
       <c r="V4" s="12"/>
     </row>
-    <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>320</v>
       </c>
@@ -884,15 +989,12 @@
         <v>321</v>
       </c>
       <c r="F5" s="11"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
       <c r="J5" s="12"/>
       <c r="L5" s="11" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="N5" s="12" t="s">
         <v>13</v>
@@ -900,6 +1002,9 @@
       <c r="O5" s="12" t="s">
         <v>10</v>
       </c>
+      <c r="P5" s="30" t="s">
+        <v>51</v>
+      </c>
       <c r="Q5" t="s">
         <v>27</v>
       </c>
@@ -917,20 +1022,17 @@
       </c>
       <c r="V5" s="12"/>
     </row>
-    <row r="6" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F6" s="11"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
       <c r="J6" s="12"/>
       <c r="L6" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="N6" s="35" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="M6" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="N6" s="28" t="s">
+        <v>38</v>
       </c>
       <c r="O6" s="12" t="s">
         <v>11</v>
@@ -939,22 +1041,18 @@
         <v>28</v>
       </c>
       <c r="R6" s="11"/>
-      <c r="S6" s="32"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="32"/>
       <c r="V6" s="12"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F7" s="11"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
       <c r="J7" s="12"/>
       <c r="L7" s="11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="M7" s="11"/>
-      <c r="N7" s="12"/>
+      <c r="N7" s="12" t="s">
+        <v>50</v>
+      </c>
       <c r="O7" s="12" t="s">
         <v>12</v>
       </c>
@@ -962,23 +1060,17 @@
         <v>29</v>
       </c>
       <c r="R7" s="11"/>
-      <c r="S7" s="32"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="32"/>
       <c r="V7" s="12"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F8" s="11"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
       <c r="J8" s="12"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
+      <c r="L8" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="N8" s="12"/>
       <c r="O8" s="12" t="s">
         <v>15</v>
@@ -987,41 +1079,28 @@
         <v>31</v>
       </c>
       <c r="R8" s="11"/>
-      <c r="S8" s="32"/>
-      <c r="T8" s="32"/>
-      <c r="U8" s="32"/>
       <c r="V8" s="12"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F9" s="11"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
       <c r="J9" s="12"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
+      <c r="L9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="N9" s="12"/>
       <c r="O9" s="12" t="s">
         <v>18</v>
       </c>
       <c r="Q9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R9" s="11"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="32"/>
-      <c r="U9" s="32"/>
       <c r="V9" s="12"/>
     </row>
-    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
+    <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F10" s="13">
         <v>76480</v>
       </c>
@@ -1031,8 +1110,12 @@
       <c r="J10" s="15">
         <v>76799</v>
       </c>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
+      <c r="L10" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="N10" s="12"/>
       <c r="O10" s="12" t="s">
         <v>19</v>
@@ -1050,17 +1133,15 @@
         <v>76799</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F11" s="16"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="17"/>
-      <c r="L11" s="11"/>
+      <c r="L11" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="M11" s="11"/>
       <c r="N11" s="12"/>
       <c r="O11" s="12" t="s">
@@ -1072,13 +1153,12 @@
       <c r="U11" s="7"/>
       <c r="V11" s="17"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F12" s="11"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
       <c r="J12" s="12"/>
-      <c r="L12" s="11"/>
+      <c r="L12" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="M12" s="11"/>
       <c r="N12" s="12"/>
       <c r="O12" s="12" t="s">
@@ -1087,13 +1167,16 @@
       <c r="R12" s="11"/>
       <c r="V12" s="12"/>
     </row>
-    <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F13" s="11"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" s="31"/>
       <c r="J13" s="12"/>
-      <c r="L13" s="11"/>
+      <c r="L13" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="M13" s="13"/>
       <c r="N13" s="15"/>
       <c r="O13" s="12" t="s">
@@ -1102,85 +1185,97 @@
       <c r="R13" s="11"/>
       <c r="V13" s="12"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F14" s="11"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14" s="31"/>
       <c r="J14" s="12"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
+      <c r="L14" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
       <c r="O14" s="12" t="s">
         <v>22</v>
       </c>
       <c r="R14" s="11"/>
       <c r="V14" s="12"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F15" s="11"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15" s="31"/>
       <c r="J15" s="12"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
+      <c r="L15" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
       <c r="O15" s="12" t="s">
         <v>23</v>
       </c>
       <c r="R15" s="11"/>
       <c r="V15" s="12"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F16" s="11"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16" s="31"/>
       <c r="J16" s="12"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
+      <c r="L16" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
       <c r="O16" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R16" s="11"/>
       <c r="V16" s="12"/>
     </row>
-    <row r="17" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F17" s="11"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
       <c r="J17" s="12"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
+      <c r="L17" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
       <c r="O17" s="12" t="s">
         <v>25</v>
       </c>
       <c r="R17" s="11"/>
       <c r="V17" s="12"/>
     </row>
-    <row r="18" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F18" s="11"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
+      <c r="H18">
+        <v>5</v>
+      </c>
       <c r="I18" s="32"/>
       <c r="J18" s="12"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
+      <c r="L18" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
       <c r="O18" s="12" t="s">
         <v>17</v>
       </c>
       <c r="R18" s="11"/>
       <c r="V18" s="12"/>
     </row>
-    <row r="19" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F19" s="11"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
+      <c r="H19">
+        <v>6</v>
+      </c>
       <c r="I19" s="32"/>
       <c r="J19" s="12"/>
       <c r="L19" s="13"/>
@@ -1192,97 +1287,161 @@
       <c r="R19" s="11"/>
       <c r="V19" s="12"/>
     </row>
-    <row r="20" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F20" s="11"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
+      <c r="H20">
+        <v>7</v>
+      </c>
       <c r="I20" s="32"/>
       <c r="J20" s="12"/>
       <c r="R20" s="11"/>
       <c r="V20" s="12"/>
     </row>
-    <row r="21" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F21" s="11"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
+      <c r="H21">
+        <v>8</v>
+      </c>
       <c r="I21" s="32"/>
       <c r="J21" s="12"/>
+      <c r="L21" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="17" t="s">
+        <v>13</v>
+      </c>
       <c r="R21" s="11"/>
       <c r="V21" s="12"/>
     </row>
-    <row r="22" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F22" s="11"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
       <c r="J22" s="12"/>
+      <c r="L22" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="12"/>
       <c r="R22" s="11"/>
       <c r="V22" s="12"/>
     </row>
-    <row r="23" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F23" s="11"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
       <c r="J23" s="12"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="N23" s="17"/>
+      <c r="O23" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="R23" s="11"/>
       <c r="V23" s="12"/>
     </row>
-    <row r="24" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F24" s="11"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
       <c r="J24" s="12"/>
+      <c r="L24" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M24" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="N24" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="O24" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="R24" s="11"/>
       <c r="V24" s="12"/>
     </row>
-    <row r="25" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:22" ht="42.75" x14ac:dyDescent="0.2">
       <c r="F25" s="11"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
       <c r="J25" s="12"/>
+      <c r="L25" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="M25" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="N25" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="O25" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="R25" s="11"/>
       <c r="V25" s="12"/>
     </row>
-    <row r="26" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F26" s="11"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
       <c r="J26" s="12"/>
+      <c r="L26" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="M26" s="11"/>
+      <c r="N26" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="O26" s="12" t="s">
+        <v>12</v>
+      </c>
       <c r="R26" s="11"/>
       <c r="V26" s="12"/>
     </row>
-    <row r="27" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F27" s="11"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
       <c r="J27" s="12"/>
+      <c r="L27" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="M27" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="R27" s="11"/>
       <c r="V27" s="12"/>
     </row>
-    <row r="28" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F28" s="11"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
       <c r="J28" s="12"/>
+      <c r="L28" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="M28" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="R28" s="11"/>
       <c r="V28" s="12"/>
     </row>
-    <row r="29" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F29" s="11"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
       <c r="J29" s="12"/>
+      <c r="L29" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="M29" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="R29" s="11"/>
       <c r="V29" s="12"/>
     </row>
-    <row r="30" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="6:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F30" s="13"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -1290,6 +1449,14 @@
       <c r="J30" s="15">
         <v>307199</v>
       </c>
+      <c r="L30" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="M30" s="11"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="R30" s="13"/>
       <c r="S30" s="14"/>
       <c r="T30" s="14"/>
@@ -1298,8 +1465,51 @@
         <v>307199</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="6:22" x14ac:dyDescent="0.2">
+      <c r="L31" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="M31" s="11"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="6:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L32" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="M32" s="13"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="R32" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="S32" s="34"/>
+      <c r="T32" s="34"/>
+      <c r="U32" s="34"/>
+      <c r="V32" s="34"/>
+    </row>
+    <row r="33" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L33" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
+      <c r="O33" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="R33" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="S33" s="34"/>
+      <c r="T33" s="34"/>
+      <c r="U33" s="34"/>
+      <c r="V33" s="34"/>
+    </row>
+    <row r="34" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>3</v>
       </c>
@@ -1313,8 +1523,21 @@
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
       <c r="J34" s="17"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L34" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="M34" s="29"/>
+      <c r="N34" s="29"/>
+      <c r="O34" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="R34" s="35"/>
+      <c r="S34" s="35"/>
+      <c r="T34" s="35"/>
+      <c r="U34" s="35"/>
+      <c r="V34" s="35"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>0</v>
       </c>
@@ -1332,8 +1555,21 @@
         <v>20</v>
       </c>
       <c r="J35" s="12"/>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L35" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="M35" s="29"/>
+      <c r="N35" s="29"/>
+      <c r="O35" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R35" s="35"/>
+      <c r="S35" s="35"/>
+      <c r="T35" s="35"/>
+      <c r="U35" s="35"/>
+      <c r="V35" s="35"/>
+    </row>
+    <row r="36" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="19">
         <v>30</v>
@@ -1349,14 +1585,40 @@
         <v>40</v>
       </c>
       <c r="J36" s="12"/>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L36" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
+      <c r="O36" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="R36" s="35"/>
+      <c r="S36" s="35"/>
+      <c r="T36" s="35"/>
+      <c r="U36" s="35"/>
+      <c r="V36" s="35"/>
+    </row>
+    <row r="37" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="E37" s="12"/>
       <c r="G37" s="11"/>
       <c r="J37" s="12"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L37" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="R37" s="35"/>
+      <c r="S37" s="35"/>
+      <c r="T37" s="35"/>
+      <c r="U37" s="35"/>
+      <c r="V37" s="35"/>
+    </row>
+    <row r="38" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>5</v>
       </c>
@@ -1384,8 +1646,14 @@
       <c r="J38" s="18">
         <v>20</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L38" s="13"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
       <c r="B39" s="22">
         <v>10</v>
@@ -1412,7 +1680,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
       <c r="B40" s="9">
         <v>30</v>
@@ -1439,7 +1707,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="19">
         <v>30</v>
@@ -1467,6 +1735,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="R32:V32"/>
+    <mergeCell ref="R33:V33"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
bram2vga.xlsx - add tasks for 7.5.25
Signed-off-by: Dvir Hershkovits <dvirhersh@gmail.com>
</commit_message>
<xml_diff>
--- a/datasheets/bram2vga.xlsx
+++ b/datasheets/bram2vga.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idowe\Projects\Digital-Zoom-FPGA\datasheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital-Zoom-FPGA\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B1431C-55A4-4C3B-B63E-0D2F81C44A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DEE517-9989-40F4-AA3C-30DAFEF7D4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9670E6A7-4A90-4DCF-AC2B-294B8B9A454C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
   <si>
     <t>BRAM</t>
   </si>
@@ -241,7 +241,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFFFF00"/>
-        <rFont val="Arial"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -251,7 +251,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -263,6 +263,51 @@
   </si>
   <si>
     <t>להתחי להרכיב את העסק</t>
+  </si>
+  <si>
+    <t>h_cnt</t>
+  </si>
+  <si>
+    <t>v_cnt</t>
+  </si>
+  <si>
+    <t>a=10</t>
+  </si>
+  <si>
+    <t>c=12</t>
+  </si>
+  <si>
+    <t>11=17</t>
+  </si>
+  <si>
+    <t>14=20</t>
+  </si>
+  <si>
+    <t>f=15</t>
+  </si>
+  <si>
+    <t>12=18</t>
+  </si>
+  <si>
+    <t>19=25</t>
+  </si>
+  <si>
+    <t>28=40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23= </t>
+  </si>
+  <si>
+    <t>tasks 7.5.25</t>
+  </si>
+  <si>
+    <t>read from correct address (addrb of 1st BRAM)</t>
+  </si>
+  <si>
+    <t>verify zoom with filter works correctly</t>
+  </si>
+  <si>
+    <t>add switch to allow without zoom &amp; zoom without filter</t>
   </si>
 </sst>
 </file>
@@ -273,20 +318,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFF00"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -347,7 +392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -435,11 +480,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -473,17 +544,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,21 +891,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05C238A-0561-4BB7-9A92-291FE0D71310}">
-  <dimension ref="A1:V41"/>
+  <dimension ref="A1:AC58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L17" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="Q35" sqref="Q35"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="12.875" customWidth="1"/>
-    <col min="12" max="13" width="23.25" customWidth="1"/>
-    <col min="16" max="16" width="30.375" customWidth="1"/>
-    <col min="17" max="17" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="47.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="12" max="13" width="23.28515625" customWidth="1"/>
+    <col min="16" max="16" width="30.42578125" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -849,7 +924,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -896,7 +971,7 @@
       </c>
       <c r="V2" s="17"/>
     </row>
-    <row r="3" spans="1:22" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -924,8 +999,6 @@
       <c r="L3" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
       <c r="O3" s="12"/>
       <c r="Q3" t="s">
         <v>30</v>
@@ -938,7 +1011,7 @@
       </c>
       <c r="V3" s="12"/>
     </row>
-    <row r="4" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>320</v>
       </c>
@@ -975,7 +1048,7 @@
       </c>
       <c r="V4" s="12"/>
     </row>
-    <row r="5" spans="1:22" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>320</v>
       </c>
@@ -1002,7 +1075,7 @@
       <c r="O5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="30" t="s">
+      <c r="P5" t="s">
         <v>51</v>
       </c>
       <c r="Q5" t="s">
@@ -1022,7 +1095,7 @@
       </c>
       <c r="V5" s="12"/>
     </row>
-    <row r="6" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="11"/>
       <c r="J6" s="12"/>
       <c r="L6" s="11" t="s">
@@ -1043,7 +1116,7 @@
       <c r="R6" s="11"/>
       <c r="V6" s="12"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F7" s="11"/>
       <c r="J7" s="12"/>
       <c r="L7" s="11" t="s">
@@ -1062,7 +1135,10 @@
       <c r="R7" s="11"/>
       <c r="V7" s="12"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
       <c r="F8" s="11"/>
       <c r="J8" s="12"/>
       <c r="L8" s="11" t="s">
@@ -1081,7 +1157,13 @@
       <c r="R8" s="11"/>
       <c r="V8" s="12"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
       <c r="F9" s="11"/>
       <c r="J9" s="12"/>
       <c r="L9" s="11" t="s">
@@ -1100,7 +1182,13 @@
       <c r="R9" s="11"/>
       <c r="V9" s="12"/>
     </row>
-    <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
       <c r="F10" s="13">
         <v>76480</v>
       </c>
@@ -1133,7 +1221,13 @@
         <v>76799</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>81</v>
+      </c>
       <c r="F11" s="16"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -1153,7 +1247,7 @@
       <c r="U11" s="7"/>
       <c r="V11" s="17"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F12" s="11"/>
       <c r="J12" s="12"/>
       <c r="L12" s="11" t="s">
@@ -1167,12 +1261,12 @@
       <c r="R12" s="11"/>
       <c r="V12" s="12"/>
     </row>
-    <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F13" s="11"/>
       <c r="H13">
         <v>1</v>
       </c>
-      <c r="I13" s="31"/>
+      <c r="I13" s="29"/>
       <c r="J13" s="12"/>
       <c r="L13" s="11" t="s">
         <v>58</v>
@@ -1185,98 +1279,88 @@
       <c r="R13" s="11"/>
       <c r="V13" s="12"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F14" s="11"/>
       <c r="H14">
         <v>2</v>
       </c>
-      <c r="I14" s="31"/>
+      <c r="I14" s="29"/>
       <c r="J14" s="12"/>
       <c r="L14" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
       <c r="O14" s="12" t="s">
         <v>22</v>
       </c>
       <c r="R14" s="11"/>
       <c r="V14" s="12"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F15" s="11"/>
       <c r="H15">
         <v>3</v>
       </c>
-      <c r="I15" s="31"/>
+      <c r="I15" s="29"/>
       <c r="J15" s="12"/>
       <c r="L15" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
       <c r="O15" s="12" t="s">
         <v>23</v>
       </c>
       <c r="R15" s="11"/>
       <c r="V15" s="12"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F16" s="11"/>
       <c r="H16">
         <v>4</v>
       </c>
-      <c r="I16" s="31"/>
+      <c r="I16" s="29"/>
       <c r="J16" s="12"/>
       <c r="L16" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
       <c r="O16" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R16" s="11"/>
       <c r="V16" s="12"/>
     </row>
-    <row r="17" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F17" s="11"/>
       <c r="J17" s="12"/>
       <c r="L17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
       <c r="O17" s="12" t="s">
         <v>25</v>
       </c>
       <c r="R17" s="11"/>
       <c r="V17" s="12"/>
     </row>
-    <row r="18" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F18" s="11"/>
       <c r="H18">
         <v>5</v>
       </c>
-      <c r="I18" s="32"/>
+      <c r="I18" s="30"/>
       <c r="J18" s="12"/>
       <c r="L18" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29"/>
       <c r="O18" s="12" t="s">
         <v>17</v>
       </c>
       <c r="R18" s="11"/>
       <c r="V18" s="12"/>
     </row>
-    <row r="19" spans="6:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="11"/>
       <c r="H19">
         <v>6</v>
       </c>
-      <c r="I19" s="32"/>
+      <c r="I19" s="30"/>
       <c r="J19" s="12"/>
       <c r="L19" s="13"/>
       <c r="M19" s="14"/>
@@ -1287,22 +1371,22 @@
       <c r="R19" s="11"/>
       <c r="V19" s="12"/>
     </row>
-    <row r="20" spans="6:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F20" s="11"/>
       <c r="H20">
         <v>7</v>
       </c>
-      <c r="I20" s="32"/>
+      <c r="I20" s="30"/>
       <c r="J20" s="12"/>
       <c r="R20" s="11"/>
       <c r="V20" s="12"/>
     </row>
-    <row r="21" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F21" s="11"/>
       <c r="H21">
         <v>8</v>
       </c>
-      <c r="I21" s="32"/>
+      <c r="I21" s="30"/>
       <c r="J21" s="12"/>
       <c r="L21" s="16" t="s">
         <v>8</v>
@@ -1315,19 +1399,17 @@
       <c r="R21" s="11"/>
       <c r="V21" s="12"/>
     </row>
-    <row r="22" spans="6:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F22" s="11"/>
       <c r="J22" s="12"/>
       <c r="L22" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29"/>
       <c r="O22" s="12"/>
       <c r="R22" s="11"/>
       <c r="V22" s="12"/>
     </row>
-    <row r="23" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F23" s="11"/>
       <c r="J23" s="12"/>
       <c r="L23" s="11"/>
@@ -1341,7 +1423,7 @@
       <c r="R23" s="11"/>
       <c r="V23" s="12"/>
     </row>
-    <row r="24" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F24" s="11"/>
       <c r="J24" s="12"/>
       <c r="L24" s="11" t="s">
@@ -1359,7 +1441,7 @@
       <c r="R24" s="11"/>
       <c r="V24" s="12"/>
     </row>
-    <row r="25" spans="6:22" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="6:22" ht="60" x14ac:dyDescent="0.25">
       <c r="F25" s="11"/>
       <c r="J25" s="12"/>
       <c r="L25" s="11" t="s">
@@ -1377,10 +1459,10 @@
       <c r="R25" s="11"/>
       <c r="V25" s="12"/>
     </row>
-    <row r="26" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F26" s="11"/>
       <c r="J26" s="12"/>
-      <c r="L26" s="33" t="s">
+      <c r="L26" s="31" t="s">
         <v>34</v>
       </c>
       <c r="M26" s="11"/>
@@ -1393,10 +1475,10 @@
       <c r="R26" s="11"/>
       <c r="V26" s="12"/>
     </row>
-    <row r="27" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F27" s="11"/>
       <c r="J27" s="12"/>
-      <c r="L27" s="33" t="s">
+      <c r="L27" s="31" t="s">
         <v>42</v>
       </c>
       <c r="M27" s="11" t="s">
@@ -1409,10 +1491,10 @@
       <c r="R27" s="11"/>
       <c r="V27" s="12"/>
     </row>
-    <row r="28" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F28" s="11"/>
       <c r="J28" s="12"/>
-      <c r="L28" s="33" t="s">
+      <c r="L28" s="31" t="s">
         <v>43</v>
       </c>
       <c r="M28" s="11" t="s">
@@ -1425,10 +1507,10 @@
       <c r="R28" s="11"/>
       <c r="V28" s="12"/>
     </row>
-    <row r="29" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F29" s="11"/>
       <c r="J29" s="12"/>
-      <c r="L29" s="33" t="s">
+      <c r="L29" s="31" t="s">
         <v>44</v>
       </c>
       <c r="M29" s="11" t="s">
@@ -1441,7 +1523,7 @@
       <c r="R29" s="11"/>
       <c r="V29" s="12"/>
     </row>
-    <row r="30" spans="6:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F30" s="13"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -1465,7 +1547,7 @@
         <v>307199</v>
       </c>
     </row>
-    <row r="31" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="6:22" x14ac:dyDescent="0.25">
       <c r="L31" s="11" t="s">
         <v>56</v>
       </c>
@@ -1475,7 +1557,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="6:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L32" s="11" t="s">
         <v>59</v>
       </c>
@@ -1484,32 +1566,30 @@
       <c r="O32" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="R32" s="34" t="s">
+      <c r="R32" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="S32" s="34"/>
-      <c r="T32" s="34"/>
-      <c r="U32" s="34"/>
-      <c r="V32" s="34"/>
-    </row>
-    <row r="33" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S32" s="33"/>
+      <c r="T32" s="33"/>
+      <c r="U32" s="33"/>
+      <c r="V32" s="33"/>
+    </row>
+    <row r="33" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L33" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="M33" s="29"/>
-      <c r="N33" s="29"/>
       <c r="O33" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="R33" s="34" t="s">
+      <c r="R33" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="S33" s="34"/>
-      <c r="T33" s="34"/>
-      <c r="U33" s="34"/>
-      <c r="V33" s="34"/>
-    </row>
-    <row r="34" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S33" s="33"/>
+      <c r="T33" s="33"/>
+      <c r="U33" s="33"/>
+      <c r="V33" s="33"/>
+    </row>
+    <row r="34" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
         <v>3</v>
       </c>
@@ -1526,18 +1606,16 @@
       <c r="L34" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="M34" s="29"/>
-      <c r="N34" s="29"/>
       <c r="O34" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="R34" s="35"/>
-      <c r="S34" s="35"/>
-      <c r="T34" s="35"/>
-      <c r="U34" s="35"/>
-      <c r="V34" s="35"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="R34" s="32"/>
+      <c r="S34" s="32"/>
+      <c r="T34" s="32"/>
+      <c r="U34" s="32"/>
+      <c r="V34" s="32"/>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>0</v>
       </c>
@@ -1558,18 +1636,16 @@
       <c r="L35" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="M35" s="29"/>
-      <c r="N35" s="29"/>
       <c r="O35" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R35" s="35"/>
-      <c r="S35" s="35"/>
-      <c r="T35" s="35"/>
-      <c r="U35" s="35"/>
-      <c r="V35" s="35"/>
-    </row>
-    <row r="36" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R35" s="32"/>
+      <c r="S35" s="32"/>
+      <c r="T35" s="32"/>
+      <c r="U35" s="32"/>
+      <c r="V35" s="32"/>
+    </row>
+    <row r="36" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
       <c r="B36" s="19">
         <v>30</v>
@@ -1588,18 +1664,16 @@
       <c r="L36" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="M36" s="29"/>
-      <c r="N36" s="29"/>
       <c r="O36" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="R36" s="35"/>
-      <c r="S36" s="35"/>
-      <c r="T36" s="35"/>
-      <c r="U36" s="35"/>
-      <c r="V36" s="35"/>
-    </row>
-    <row r="37" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R36" s="32"/>
+      <c r="S36" s="32"/>
+      <c r="T36" s="32"/>
+      <c r="U36" s="32"/>
+      <c r="V36" s="32"/>
+    </row>
+    <row r="37" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11"/>
       <c r="E37" s="12"/>
       <c r="G37" s="11"/>
@@ -1607,18 +1681,16 @@
       <c r="L37" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
       <c r="O37" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="R37" s="35"/>
-      <c r="S37" s="35"/>
-      <c r="T37" s="35"/>
-      <c r="U37" s="35"/>
-      <c r="V37" s="35"/>
-    </row>
-    <row r="38" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R37" s="32"/>
+      <c r="S37" s="32"/>
+      <c r="T37" s="32"/>
+      <c r="U37" s="32"/>
+      <c r="V37" s="32"/>
+    </row>
+    <row r="38" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>5</v>
       </c>
@@ -1653,7 +1725,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="22">
         <v>10</v>
@@ -1680,7 +1752,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="9">
         <v>30</v>
@@ -1707,7 +1779,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
       <c r="B41" s="19">
         <v>30</v>
@@ -1733,6 +1805,228 @@
       <c r="J41" s="20">
         <v>40</v>
       </c>
+    </row>
+    <row r="42" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="G43" s="18">
+        <v>20</v>
+      </c>
+      <c r="H43">
+        <f>G43+(J43-G43)/3</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="J43" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="I46" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="J46" s="16">
+        <v>0</v>
+      </c>
+      <c r="K46" s="7">
+        <v>1</v>
+      </c>
+      <c r="L46" s="7">
+        <v>2</v>
+      </c>
+      <c r="M46" s="17">
+        <v>3</v>
+      </c>
+      <c r="N46" s="16">
+        <v>0</v>
+      </c>
+      <c r="O46" s="7">
+        <v>1</v>
+      </c>
+      <c r="P46" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q46" s="17">
+        <v>3</v>
+      </c>
+      <c r="R46" s="16">
+        <v>0</v>
+      </c>
+      <c r="S46" s="7">
+        <v>1</v>
+      </c>
+      <c r="T46" s="7">
+        <v>2</v>
+      </c>
+      <c r="U46" s="17">
+        <v>3</v>
+      </c>
+      <c r="V46" s="16">
+        <v>0</v>
+      </c>
+      <c r="W46" s="7">
+        <v>1</v>
+      </c>
+      <c r="X46" s="7">
+        <v>2</v>
+      </c>
+      <c r="Y46" s="17">
+        <v>3</v>
+      </c>
+      <c r="Z46" s="36">
+        <v>4</v>
+      </c>
+      <c r="AA46" s="36">
+        <v>5</v>
+      </c>
+      <c r="AB46" s="36">
+        <v>6</v>
+      </c>
+      <c r="AC46" s="36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I47" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J47" s="13">
+        <v>0</v>
+      </c>
+      <c r="K47" s="14">
+        <v>0</v>
+      </c>
+      <c r="L47" s="14">
+        <v>0</v>
+      </c>
+      <c r="M47" s="15">
+        <v>0</v>
+      </c>
+      <c r="N47" s="13">
+        <v>1</v>
+      </c>
+      <c r="O47" s="14">
+        <v>1</v>
+      </c>
+      <c r="P47" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="15">
+        <v>1</v>
+      </c>
+      <c r="R47" s="13">
+        <v>2</v>
+      </c>
+      <c r="S47" s="14">
+        <v>2</v>
+      </c>
+      <c r="T47" s="14">
+        <v>2</v>
+      </c>
+      <c r="U47" s="15">
+        <v>2</v>
+      </c>
+      <c r="V47" s="13">
+        <v>3</v>
+      </c>
+      <c r="W47" s="14">
+        <v>3</v>
+      </c>
+      <c r="X47" s="14">
+        <v>3</v>
+      </c>
+      <c r="Y47" s="15">
+        <v>3</v>
+      </c>
+      <c r="Z47" s="36">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="36">
+        <v>0</v>
+      </c>
+      <c r="AB47" s="36">
+        <v>0</v>
+      </c>
+      <c r="AC47" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D50" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G50" s="18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D51" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E51" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F51" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D52" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E52" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="F52" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D53" s="25">
+        <v>30</v>
+      </c>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D55" s="16"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="17"/>
+    </row>
+    <row r="56" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D56" s="11"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="12"/>
+    </row>
+    <row r="57" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D57" s="11"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="12"/>
+    </row>
+    <row r="58" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D58" s="13"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
bili top - need to keep working on its simulation - sync address_write with pixel_out and wr_en..
Signed-off-by: idowein <ido.weinstock@gmail.com>
</commit_message>
<xml_diff>
--- a/datasheets/bram2vga.xlsx
+++ b/datasheets/bram2vga.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idowe\Projects\Digital-Zoom-FPGA\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766CE74E-37FE-40E2-ACF5-004537AA0A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC8DFA5-46EA-4BFD-AB16-2018F90E7FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9670E6A7-4A90-4DCF-AC2B-294B8B9A454C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="77">
   <si>
     <t>BRAM</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>utilize BILI - simulation + chip scope (?)</t>
+  </si>
+  <si>
+    <t>sync address write with pixel_out and wr_en, ask ori if wr_en = 1 is healthy..</t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -512,11 +515,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05C238A-0561-4BB7-9A92-291FE0D71310}">
-  <dimension ref="A1:V47"/>
+  <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1121,11 +1123,11 @@
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
       <c r="F9" s="11"/>
       <c r="J9" s="12"/>
       <c r="L9" s="11" t="s">
@@ -1189,11 +1191,11 @@
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
       <c r="F11" s="16"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -1346,6 +1348,12 @@
       <c r="V18" s="12"/>
     </row>
     <row r="19" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
       <c r="F19" s="11"/>
       <c r="H19">
         <v>6</v>
@@ -1556,13 +1564,13 @@
       <c r="O32" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="R32" s="33" t="s">
+      <c r="R32" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="S32" s="33"/>
-      <c r="T32" s="33"/>
-      <c r="U32" s="33"/>
-      <c r="V32" s="33"/>
+      <c r="S32" s="34"/>
+      <c r="T32" s="34"/>
+      <c r="U32" s="34"/>
+      <c r="V32" s="34"/>
     </row>
     <row r="33" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L33" s="11" t="s">
@@ -1571,13 +1579,13 @@
       <c r="O33" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="R33" s="33" t="s">
+      <c r="R33" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="S33" s="33"/>
-      <c r="T33" s="33"/>
-      <c r="U33" s="33"/>
-      <c r="V33" s="33"/>
+      <c r="S33" s="34"/>
+      <c r="T33" s="34"/>
+      <c r="U33" s="34"/>
+      <c r="V33" s="34"/>
     </row>
     <row r="34" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
@@ -1808,24 +1816,6 @@
       <c r="J43" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="35"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
BILINEAR_INTERPOLATION_TOP.vhd - align address_write & wr_en to pixel_out - bili_cntl - still creates a blur video
Signed-off-by: idowein <ido.weinstock@gmail.com>
</commit_message>
<xml_diff>
--- a/datasheets/bram2vga.xlsx
+++ b/datasheets/bram2vga.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idowe\Projects\Digital-Zoom-FPGA\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC8DFA5-46EA-4BFD-AB16-2018F90E7FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B21272F-BC11-4F62-8C44-EE646499CB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9670E6A7-4A90-4DCF-AC2B-294B8B9A454C}"/>
   </bookViews>
@@ -855,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05C238A-0561-4BB7-9A92-291FE0D71310}">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
changing bil clk 100 MHZ to 50 MHZ .
Signed-off-by: idowein <ido.weinstock@gmail.com>
</commit_message>
<xml_diff>
--- a/datasheets/bram2vga.xlsx
+++ b/datasheets/bram2vga.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idowe\Projects\Digital-Zoom-FPGA\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B21272F-BC11-4F62-8C44-EE646499CB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE93C495-AEC7-43CA-931D-975218850F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9670E6A7-4A90-4DCF-AC2B-294B8B9A454C}"/>
   </bookViews>
@@ -856,7 +856,7 @@
   <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
modifying camera datasheet .txt
Signed-off-by: idowein <ido.weinstock@gmail.com>
</commit_message>
<xml_diff>
--- a/datasheets/bram2vga.xlsx
+++ b/datasheets/bram2vga.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital-Zoom-FPGA\datasheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idowe\Projects\Digital-Zoom-FPGA\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DEE517-9989-40F4-AA3C-30DAFEF7D4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE93C495-AEC7-43CA-931D-975218850F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9670E6A7-4A90-4DCF-AC2B-294B8B9A454C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="77">
   <si>
     <t>BRAM</t>
   </si>
@@ -241,7 +241,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFFFF00"/>
-        <rFont val="Aptos Narrow"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -251,7 +251,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -265,39 +265,6 @@
     <t>להתחי להרכיב את העסק</t>
   </si>
   <si>
-    <t>h_cnt</t>
-  </si>
-  <si>
-    <t>v_cnt</t>
-  </si>
-  <si>
-    <t>a=10</t>
-  </si>
-  <si>
-    <t>c=12</t>
-  </si>
-  <si>
-    <t>11=17</t>
-  </si>
-  <si>
-    <t>14=20</t>
-  </si>
-  <si>
-    <t>f=15</t>
-  </si>
-  <si>
-    <t>12=18</t>
-  </si>
-  <si>
-    <t>19=25</t>
-  </si>
-  <si>
-    <t>28=40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23= </t>
-  </si>
-  <si>
     <t>tasks 7.5.25</t>
   </si>
   <si>
@@ -308,6 +275,24 @@
   </si>
   <si>
     <t>add switch to allow without zoom &amp; zoom without filter</t>
+  </si>
+  <si>
+    <t>tasks 8.5.25</t>
+  </si>
+  <si>
+    <t>utilize regular zoom as in tag "system_works_2_BRAM</t>
+  </si>
+  <si>
+    <t>understand better the wr_en for BILI - should it be all the time?!</t>
+  </si>
+  <si>
+    <t>why wr_en in capture is 25MHz / 2 (yemeni's step")?</t>
+  </si>
+  <si>
+    <t>utilize BILI - simulation + chip scope (?)</t>
+  </si>
+  <si>
+    <t>sync address write with pixel_out and wr_en, ask ori if wr_en = 1 is healthy..</t>
   </si>
 </sst>
 </file>
@@ -318,25 +303,25 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFF00"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,8 +376,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -480,37 +471,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -550,13 +515,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -891,23 +853,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05C238A-0561-4BB7-9A92-291FE0D71310}">
-  <dimension ref="A1:AC58"/>
+  <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="47.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" customWidth="1"/>
-    <col min="12" max="13" width="23.28515625" customWidth="1"/>
-    <col min="16" max="16" width="30.42578125" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="47.625" customWidth="1"/>
+    <col min="11" max="11" width="12.875" customWidth="1"/>
+    <col min="12" max="13" width="23.25" customWidth="1"/>
+    <col min="16" max="16" width="30.375" customWidth="1"/>
+    <col min="17" max="17" width="11.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -924,7 +886,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -971,7 +933,7 @@
       </c>
       <c r="V2" s="17"/>
     </row>
-    <row r="3" spans="1:22" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -1011,7 +973,7 @@
       </c>
       <c r="V3" s="12"/>
     </row>
-    <row r="4" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>320</v>
       </c>
@@ -1048,7 +1010,7 @@
       </c>
       <c r="V4" s="12"/>
     </row>
-    <row r="5" spans="1:22" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>320</v>
       </c>
@@ -1095,7 +1057,7 @@
       </c>
       <c r="V5" s="12"/>
     </row>
-    <row r="6" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F6" s="11"/>
       <c r="J6" s="12"/>
       <c r="L6" s="11" t="s">
@@ -1116,7 +1078,7 @@
       <c r="R6" s="11"/>
       <c r="V6" s="12"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F7" s="11"/>
       <c r="J7" s="12"/>
       <c r="L7" s="11" t="s">
@@ -1135,9 +1097,9 @@
       <c r="R7" s="11"/>
       <c r="V7" s="12"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="F8" s="11"/>
       <c r="J8" s="12"/>
@@ -1157,13 +1119,15 @@
       <c r="R8" s="11"/>
       <c r="V8" s="12"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
-        <v>79</v>
-      </c>
+      <c r="B9" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
       <c r="F9" s="11"/>
       <c r="J9" s="12"/>
       <c r="L9" s="11" t="s">
@@ -1182,13 +1146,15 @@
       <c r="R9" s="11"/>
       <c r="V9" s="12"/>
     </row>
-    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
-        <v>80</v>
-      </c>
+      <c r="B10" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
       <c r="F10" s="13">
         <v>76480</v>
       </c>
@@ -1221,13 +1187,15 @@
         <v>76799</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="B11" t="s">
-        <v>81</v>
-      </c>
+      <c r="B11" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
       <c r="F11" s="16"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -1247,7 +1215,7 @@
       <c r="U11" s="7"/>
       <c r="V11" s="17"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F12" s="11"/>
       <c r="J12" s="12"/>
       <c r="L12" s="11" t="s">
@@ -1261,7 +1229,10 @@
       <c r="R12" s="11"/>
       <c r="V12" s="12"/>
     </row>
-    <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
       <c r="F13" s="11"/>
       <c r="H13">
         <v>1</v>
@@ -1279,7 +1250,13 @@
       <c r="R13" s="11"/>
       <c r="V13" s="12"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
       <c r="F14" s="11"/>
       <c r="H14">
         <v>2</v>
@@ -1295,7 +1272,13 @@
       <c r="R14" s="11"/>
       <c r="V14" s="12"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
       <c r="F15" s="11"/>
       <c r="H15">
         <v>3</v>
@@ -1311,7 +1294,10 @@
       <c r="R15" s="11"/>
       <c r="V15" s="12"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
       <c r="F16" s="11"/>
       <c r="H16">
         <v>4</v>
@@ -1327,7 +1313,13 @@
       <c r="R16" s="11"/>
       <c r="V16" s="12"/>
     </row>
-    <row r="17" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
       <c r="F17" s="11"/>
       <c r="J17" s="12"/>
       <c r="L17" s="11" t="s">
@@ -1339,7 +1331,7 @@
       <c r="R17" s="11"/>
       <c r="V17" s="12"/>
     </row>
-    <row r="18" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F18" s="11"/>
       <c r="H18">
         <v>5</v>
@@ -1355,7 +1347,13 @@
       <c r="R18" s="11"/>
       <c r="V18" s="12"/>
     </row>
-    <row r="19" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
       <c r="F19" s="11"/>
       <c r="H19">
         <v>6</v>
@@ -1371,7 +1369,7 @@
       <c r="R19" s="11"/>
       <c r="V19" s="12"/>
     </row>
-    <row r="20" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F20" s="11"/>
       <c r="H20">
         <v>7</v>
@@ -1381,7 +1379,7 @@
       <c r="R20" s="11"/>
       <c r="V20" s="12"/>
     </row>
-    <row r="21" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F21" s="11"/>
       <c r="H21">
         <v>8</v>
@@ -1399,7 +1397,7 @@
       <c r="R21" s="11"/>
       <c r="V21" s="12"/>
     </row>
-    <row r="22" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F22" s="11"/>
       <c r="J22" s="12"/>
       <c r="L22" s="27" t="s">
@@ -1409,7 +1407,7 @@
       <c r="R22" s="11"/>
       <c r="V22" s="12"/>
     </row>
-    <row r="23" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F23" s="11"/>
       <c r="J23" s="12"/>
       <c r="L23" s="11"/>
@@ -1423,7 +1421,7 @@
       <c r="R23" s="11"/>
       <c r="V23" s="12"/>
     </row>
-    <row r="24" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F24" s="11"/>
       <c r="J24" s="12"/>
       <c r="L24" s="11" t="s">
@@ -1441,7 +1439,7 @@
       <c r="R24" s="11"/>
       <c r="V24" s="12"/>
     </row>
-    <row r="25" spans="6:22" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" ht="42.75" x14ac:dyDescent="0.2">
       <c r="F25" s="11"/>
       <c r="J25" s="12"/>
       <c r="L25" s="11" t="s">
@@ -1459,7 +1457,7 @@
       <c r="R25" s="11"/>
       <c r="V25" s="12"/>
     </row>
-    <row r="26" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F26" s="11"/>
       <c r="J26" s="12"/>
       <c r="L26" s="31" t="s">
@@ -1475,7 +1473,7 @@
       <c r="R26" s="11"/>
       <c r="V26" s="12"/>
     </row>
-    <row r="27" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F27" s="11"/>
       <c r="J27" s="12"/>
       <c r="L27" s="31" t="s">
@@ -1491,7 +1489,7 @@
       <c r="R27" s="11"/>
       <c r="V27" s="12"/>
     </row>
-    <row r="28" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F28" s="11"/>
       <c r="J28" s="12"/>
       <c r="L28" s="31" t="s">
@@ -1507,7 +1505,7 @@
       <c r="R28" s="11"/>
       <c r="V28" s="12"/>
     </row>
-    <row r="29" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F29" s="11"/>
       <c r="J29" s="12"/>
       <c r="L29" s="31" t="s">
@@ -1523,7 +1521,7 @@
       <c r="R29" s="11"/>
       <c r="V29" s="12"/>
     </row>
-    <row r="30" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F30" s="13"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -1547,7 +1545,7 @@
         <v>307199</v>
       </c>
     </row>
-    <row r="31" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="L31" s="11" t="s">
         <v>56</v>
       </c>
@@ -1557,7 +1555,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L32" s="11" t="s">
         <v>59</v>
       </c>
@@ -1566,30 +1564,30 @@
       <c r="O32" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="R32" s="33" t="s">
+      <c r="R32" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="S32" s="33"/>
-      <c r="T32" s="33"/>
-      <c r="U32" s="33"/>
-      <c r="V32" s="33"/>
-    </row>
-    <row r="33" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S32" s="34"/>
+      <c r="T32" s="34"/>
+      <c r="U32" s="34"/>
+      <c r="V32" s="34"/>
+    </row>
+    <row r="33" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L33" s="11" t="s">
         <v>63</v>
       </c>
       <c r="O33" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="R33" s="33" t="s">
+      <c r="R33" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="S33" s="33"/>
-      <c r="T33" s="33"/>
-      <c r="U33" s="33"/>
-      <c r="V33" s="33"/>
-    </row>
-    <row r="34" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S33" s="34"/>
+      <c r="T33" s="34"/>
+      <c r="U33" s="34"/>
+      <c r="V33" s="34"/>
+    </row>
+    <row r="34" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>3</v>
       </c>
@@ -1615,7 +1613,7 @@
       <c r="U34" s="32"/>
       <c r="V34" s="32"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>0</v>
       </c>
@@ -1645,7 +1643,7 @@
       <c r="U35" s="32"/>
       <c r="V35" s="32"/>
     </row>
-    <row r="36" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="19">
         <v>30</v>
@@ -1673,7 +1671,7 @@
       <c r="U36" s="32"/>
       <c r="V36" s="32"/>
     </row>
-    <row r="37" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="E37" s="12"/>
       <c r="G37" s="11"/>
@@ -1690,7 +1688,7 @@
       <c r="U37" s="32"/>
       <c r="V37" s="32"/>
     </row>
-    <row r="38" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>5</v>
       </c>
@@ -1725,7 +1723,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
       <c r="B39" s="22">
         <v>10</v>
@@ -1752,7 +1750,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
       <c r="B40" s="9">
         <v>30</v>
@@ -1779,7 +1777,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="19">
         <v>30</v>
@@ -1806,8 +1804,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G43" s="18">
         <v>20</v>
       </c>
@@ -1818,215 +1816,6 @@
       <c r="J43" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="I46" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="J46" s="16">
-        <v>0</v>
-      </c>
-      <c r="K46" s="7">
-        <v>1</v>
-      </c>
-      <c r="L46" s="7">
-        <v>2</v>
-      </c>
-      <c r="M46" s="17">
-        <v>3</v>
-      </c>
-      <c r="N46" s="16">
-        <v>0</v>
-      </c>
-      <c r="O46" s="7">
-        <v>1</v>
-      </c>
-      <c r="P46" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q46" s="17">
-        <v>3</v>
-      </c>
-      <c r="R46" s="16">
-        <v>0</v>
-      </c>
-      <c r="S46" s="7">
-        <v>1</v>
-      </c>
-      <c r="T46" s="7">
-        <v>2</v>
-      </c>
-      <c r="U46" s="17">
-        <v>3</v>
-      </c>
-      <c r="V46" s="16">
-        <v>0</v>
-      </c>
-      <c r="W46" s="7">
-        <v>1</v>
-      </c>
-      <c r="X46" s="7">
-        <v>2</v>
-      </c>
-      <c r="Y46" s="17">
-        <v>3</v>
-      </c>
-      <c r="Z46" s="36">
-        <v>4</v>
-      </c>
-      <c r="AA46" s="36">
-        <v>5</v>
-      </c>
-      <c r="AB46" s="36">
-        <v>6</v>
-      </c>
-      <c r="AC46" s="36">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I47" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="J47" s="13">
-        <v>0</v>
-      </c>
-      <c r="K47" s="14">
-        <v>0</v>
-      </c>
-      <c r="L47" s="14">
-        <v>0</v>
-      </c>
-      <c r="M47" s="15">
-        <v>0</v>
-      </c>
-      <c r="N47" s="13">
-        <v>1</v>
-      </c>
-      <c r="O47" s="14">
-        <v>1</v>
-      </c>
-      <c r="P47" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q47" s="15">
-        <v>1</v>
-      </c>
-      <c r="R47" s="13">
-        <v>2</v>
-      </c>
-      <c r="S47" s="14">
-        <v>2</v>
-      </c>
-      <c r="T47" s="14">
-        <v>2</v>
-      </c>
-      <c r="U47" s="15">
-        <v>2</v>
-      </c>
-      <c r="V47" s="13">
-        <v>3</v>
-      </c>
-      <c r="W47" s="14">
-        <v>3</v>
-      </c>
-      <c r="X47" s="14">
-        <v>3</v>
-      </c>
-      <c r="Y47" s="15">
-        <v>3</v>
-      </c>
-      <c r="Z47" s="36">
-        <v>0</v>
-      </c>
-      <c r="AA47" s="36">
-        <v>0</v>
-      </c>
-      <c r="AB47" s="36">
-        <v>0</v>
-      </c>
-      <c r="AC47" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D50" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G50" s="18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="51" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D51" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E51" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="F51" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="52" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D52" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E52" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="F52" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="G52" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="53" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="25">
-        <v>30</v>
-      </c>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="54" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D55" s="16"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="17"/>
-    </row>
-    <row r="56" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D56" s="11"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="12"/>
-    </row>
-    <row r="57" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D57" s="11"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="37"/>
-      <c r="G57" s="12"/>
-    </row>
-    <row r="58" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D58" s="13"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
fix simulation for BILI
Signed-off-by: idowein <ido.weinstock@gmail.com>
</commit_message>
<xml_diff>
--- a/datasheets/bram2vga.xlsx
+++ b/datasheets/bram2vga.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idowe\Projects\Digital-Zoom-FPGA\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE93C495-AEC7-43CA-931D-975218850F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71444345-1000-4B83-8200-44C7E231B966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9670E6A7-4A90-4DCF-AC2B-294B8B9A454C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
   <si>
     <t>BRAM</t>
   </si>
@@ -143,30 +143,12 @@
     <t xml:space="preserve">pix1 - 0 </t>
   </si>
   <si>
-    <t>BILI_big</t>
-  </si>
-  <si>
-    <t>BILI_small</t>
-  </si>
-  <si>
-    <t>clk_bili_small
-6.25MHz
-(160nS)</t>
-  </si>
-  <si>
-    <t>16 pixels
-(after time calc)</t>
-  </si>
-  <si>
     <t>clka - 25 mhz</t>
   </si>
   <si>
     <t>clkb - 25 mhz</t>
   </si>
   <si>
-    <t>clk_bili_big_ 25 mhz</t>
-  </si>
-  <si>
     <t>pix2 - 40 ns</t>
   </si>
   <si>
@@ -176,24 +158,6 @@
     <t>pix4 - 120</t>
   </si>
   <si>
-    <t>clk_bili_small 5mhz</t>
-  </si>
-  <si>
-    <t>Example:</t>
-  </si>
-  <si>
-    <t>4 pixels - 120 ns</t>
-  </si>
-  <si>
-    <t>Round 1</t>
-  </si>
-  <si>
-    <t>output - 360 ns (After one 5mhz clock)</t>
-  </si>
-  <si>
-    <t>5 mhz</t>
-  </si>
-  <si>
     <t>( 200 ns / 16 px ) = 12.5 ns -&gt; 80 mhz</t>
   </si>
   <si>
@@ -203,9 +167,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">pix 4 - 280 </t>
-  </si>
-  <si>
     <t>output to small bili - 320</t>
   </si>
   <si>
@@ -218,47 +179,9 @@
     <t>pix 7 &amp; output x 4 - 240</t>
   </si>
   <si>
-    <t>pix 7  - 240</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clk_bili_small
-</t>
-  </si>
-  <si>
-    <t>clk_bili_small 6.25mhz</t>
-  </si>
-  <si>
-    <t>100 mhz</t>
-  </si>
-  <si>
     <t xml:space="preserve">pix 8 - 280 </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">pix 5 &amp; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>output x 4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - 160</t>
-    </r>
-  </si>
-  <si>
     <t>לחשב בלי אנסיינגד אלא עם דאון-טו</t>
   </si>
   <si>
@@ -293,6 +216,33 @@
   </si>
   <si>
     <t>sync address write with pixel_out and wr_en, ask ori if wr_en = 1 is healthy..</t>
+  </si>
+  <si>
+    <t>clka = 25Mhz</t>
+  </si>
+  <si>
+    <t>wr_en toggles</t>
+  </si>
+  <si>
+    <t>actual write - 12.5MHz</t>
+  </si>
+  <si>
+    <t>clk_vga - 25</t>
+  </si>
+  <si>
+    <t>clk_interpolation - 6.25</t>
+  </si>
+  <si>
+    <t>clk_bili_wr - 50 mhz</t>
+  </si>
+  <si>
+    <t>BILI_top</t>
+  </si>
+  <si>
+    <t>pixel_out</t>
+  </si>
+  <si>
+    <t>pixel_in - 25 mhz (40 ns)</t>
   </si>
 </sst>
 </file>
@@ -314,14 +264,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFF00"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,6 +330,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -506,18 +463,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -856,31 +815,45 @@
   <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="14.375" customWidth="1"/>
     <col min="4" max="4" width="47.625" customWidth="1"/>
-    <col min="11" max="11" width="12.875" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
     <col min="12" max="13" width="23.25" customWidth="1"/>
     <col min="16" max="16" width="30.375" customWidth="1"/>
     <col min="17" max="17" width="11.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="33" t="s">
         <v>6</v>
       </c>
+      <c r="G1" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>62</v>
+      </c>
       <c r="M1" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="R1" t="s">
         <v>7</v>
@@ -933,7 +906,7 @@
       </c>
       <c r="V2" s="17"/>
     </row>
-    <row r="3" spans="1:22" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -956,11 +929,13 @@
         <v>639</v>
       </c>
       <c r="K3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L3" s="27" t="s">
-        <v>41</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
       <c r="O3" s="12"/>
       <c r="Q3" t="s">
         <v>30</v>
@@ -989,18 +964,18 @@
       <c r="F4" s="11"/>
       <c r="J4" s="12"/>
       <c r="K4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="17"/>
-      <c r="O4" s="12" t="s">
+      <c r="L4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35" t="s">
         <v>9</v>
       </c>
+      <c r="O4" s="12"/>
       <c r="Q4" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="R4" s="11">
         <v>210</v>
@@ -1026,19 +1001,15 @@
       <c r="F5" s="11"/>
       <c r="J5" s="12"/>
       <c r="L5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35" t="s">
         <v>10</v>
       </c>
+      <c r="O5" s="12"/>
       <c r="P5" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="Q5" t="s">
         <v>27</v>
@@ -1061,17 +1032,13 @@
       <c r="F6" s="11"/>
       <c r="J6" s="12"/>
       <c r="L6" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M6" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="N6" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" s="36"/>
+      <c r="N6" s="35" t="s">
         <v>11</v>
       </c>
+      <c r="O6" s="12"/>
       <c r="Q6" t="s">
         <v>28</v>
       </c>
@@ -1082,15 +1049,15 @@
       <c r="F7" s="11"/>
       <c r="J7" s="12"/>
       <c r="L7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="11"/>
-      <c r="N7" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="O7" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="35" t="s">
         <v>12</v>
       </c>
+      <c r="O7" s="12"/>
       <c r="Q7" t="s">
         <v>29</v>
       </c>
@@ -1099,20 +1066,20 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="F8" s="11"/>
       <c r="J8" s="12"/>
       <c r="L8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="M8" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12" t="s">
+      <c r="M8" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" s="35" t="s">
         <v>15</v>
       </c>
+      <c r="O8" s="12"/>
       <c r="Q8" t="s">
         <v>31</v>
       </c>
@@ -1123,23 +1090,21 @@
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
+      <c r="B9" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
       <c r="F9" s="11"/>
       <c r="J9" s="12"/>
-      <c r="L9" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12" t="s">
+      <c r="L9" s="11"/>
+      <c r="M9" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="N9" s="35" t="s">
         <v>18</v>
       </c>
+      <c r="O9" s="12"/>
       <c r="Q9" t="s">
         <v>33</v>
       </c>
@@ -1150,11 +1115,11 @@
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
+      <c r="B10" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
       <c r="F10" s="13">
         <v>76480</v>
       </c>
@@ -1165,14 +1130,16 @@
         <v>76799</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="N10" s="12"/>
+        <v>68</v>
+      </c>
+      <c r="M10" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="N10" s="35" t="s">
+        <v>19</v>
+      </c>
       <c r="O10" s="12" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="Q10" t="s">
         <v>32</v>
@@ -1191,24 +1158,24 @@
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="B11" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
+      <c r="B11" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
       <c r="F11" s="16"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="17"/>
-      <c r="L11" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="M11" s="11"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12" t="s">
+      <c r="L11" s="11"/>
+      <c r="M11" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="N11" s="35" t="s">
         <v>20</v>
       </c>
+      <c r="O11" s="12"/>
       <c r="R11" s="16"/>
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
@@ -1218,35 +1185,35 @@
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F12" s="11"/>
       <c r="J12" s="12"/>
-      <c r="L12" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="M12" s="11"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12" t="s">
+      <c r="L12" s="11"/>
+      <c r="M12" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="35" t="s">
         <v>16</v>
       </c>
+      <c r="O12" s="12"/>
       <c r="R12" s="11"/>
       <c r="V12" s="12"/>
     </row>
-    <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="F13" s="11"/>
       <c r="H13">
         <v>1</v>
       </c>
-      <c r="I13" s="29"/>
+      <c r="I13" s="28"/>
       <c r="J13" s="12"/>
-      <c r="L13" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="M13" s="13"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="12" t="s">
+      <c r="L13" s="11"/>
+      <c r="M13" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="N13" s="35" t="s">
         <v>21</v>
       </c>
+      <c r="O13" s="12"/>
       <c r="R13" s="11"/>
       <c r="V13" s="12"/>
     </row>
@@ -1255,20 +1222,22 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="F14" s="11"/>
       <c r="H14">
         <v>2</v>
       </c>
-      <c r="I14" s="29"/>
+      <c r="I14" s="28"/>
       <c r="J14" s="12"/>
-      <c r="L14" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="O14" s="12" t="s">
+      <c r="L14" s="11"/>
+      <c r="M14" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="N14" s="35" t="s">
         <v>22</v>
       </c>
+      <c r="O14" s="12"/>
       <c r="R14" s="11"/>
       <c r="V14" s="12"/>
     </row>
@@ -1277,39 +1246,43 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="F15" s="11"/>
       <c r="H15">
         <v>3</v>
       </c>
-      <c r="I15" s="29"/>
+      <c r="I15" s="28"/>
       <c r="J15" s="12"/>
-      <c r="L15" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="O15" s="12" t="s">
+      <c r="L15" s="11"/>
+      <c r="M15" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="N15" s="35" t="s">
         <v>23</v>
       </c>
+      <c r="O15" s="12"/>
       <c r="R15" s="11"/>
       <c r="V15" s="12"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="F16" s="11"/>
       <c r="H16">
         <v>4</v>
       </c>
-      <c r="I16" s="29"/>
+      <c r="I16" s="28"/>
       <c r="J16" s="12"/>
-      <c r="L16" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="O16" s="12" t="s">
+      <c r="L16" s="11"/>
+      <c r="M16" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="N16" s="35" t="s">
         <v>24</v>
       </c>
+      <c r="O16" s="12"/>
       <c r="R16" s="11"/>
       <c r="V16" s="12"/>
     </row>
@@ -1318,16 +1291,16 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="F17" s="11"/>
       <c r="J17" s="12"/>
-      <c r="L17" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="O17" s="12" t="s">
+      <c r="L17" s="11"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35" t="s">
         <v>25</v>
       </c>
+      <c r="O17" s="12"/>
       <c r="R17" s="11"/>
       <c r="V17" s="12"/>
     </row>
@@ -1336,14 +1309,14 @@
       <c r="H18">
         <v>5</v>
       </c>
-      <c r="I18" s="30"/>
+      <c r="I18" s="29"/>
       <c r="J18" s="12"/>
-      <c r="L18" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="O18" s="12" t="s">
+      <c r="L18" s="11"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35" t="s">
         <v>17</v>
       </c>
+      <c r="O18" s="12"/>
       <c r="R18" s="11"/>
       <c r="V18" s="12"/>
     </row>
@@ -1352,29 +1325,29 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="F19" s="11"/>
       <c r="H19">
         <v>6</v>
       </c>
-      <c r="I19" s="30"/>
+      <c r="I19" s="29"/>
       <c r="J19" s="12"/>
       <c r="L19" s="13"/>
       <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="15" t="s">
+      <c r="N19" s="14" t="s">
         <v>14</v>
       </c>
+      <c r="O19" s="15"/>
       <c r="R19" s="11"/>
       <c r="V19" s="12"/>
     </row>
-    <row r="20" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F20" s="11"/>
       <c r="H20">
         <v>7</v>
       </c>
-      <c r="I20" s="30"/>
+      <c r="I20" s="29"/>
       <c r="J20" s="12"/>
       <c r="R20" s="11"/>
       <c r="V20" s="12"/>
@@ -1384,140 +1357,92 @@
       <c r="H21">
         <v>8</v>
       </c>
-      <c r="I21" s="30"/>
+      <c r="I21" s="29"/>
       <c r="J21" s="12"/>
-      <c r="L21" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="17" t="s">
-        <v>13</v>
-      </c>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
       <c r="R21" s="11"/>
       <c r="V21" s="12"/>
     </row>
-    <row r="22" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F22" s="11"/>
       <c r="J22" s="12"/>
-      <c r="L22" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="O22" s="12"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="35"/>
       <c r="R22" s="11"/>
       <c r="V22" s="12"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F23" s="11"/>
       <c r="J23" s="12"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="N23" s="17"/>
-      <c r="O23" s="12" t="s">
-        <v>9</v>
-      </c>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="35"/>
       <c r="R23" s="11"/>
       <c r="V23" s="12"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F24" s="11"/>
       <c r="J24" s="12"/>
-      <c r="L24" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="M24" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="N24" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="O24" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
       <c r="R24" s="11"/>
       <c r="V24" s="12"/>
     </row>
-    <row r="25" spans="1:22" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F25" s="11"/>
       <c r="J25" s="12"/>
-      <c r="L25" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M25" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="N25" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="O25" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="L25" s="35"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="35"/>
       <c r="R25" s="11"/>
       <c r="V25" s="12"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F26" s="11"/>
       <c r="J26" s="12"/>
-      <c r="L26" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="M26" s="11"/>
-      <c r="N26" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="O26" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
       <c r="R26" s="11"/>
       <c r="V26" s="12"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F27" s="11"/>
       <c r="J27" s="12"/>
-      <c r="L27" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="M27" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="L27" s="35"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="35"/>
       <c r="R27" s="11"/>
       <c r="V27" s="12"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F28" s="11"/>
       <c r="J28" s="12"/>
-      <c r="L28" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="M28" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="L28" s="36"/>
+      <c r="M28" s="35"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="35"/>
       <c r="R28" s="11"/>
       <c r="V28" s="12"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F29" s="11"/>
       <c r="J29" s="12"/>
-      <c r="L29" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="M29" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="L29" s="35"/>
+      <c r="M29" s="35"/>
+      <c r="N29" s="35"/>
+      <c r="O29" s="35"/>
       <c r="R29" s="11"/>
       <c r="V29" s="12"/>
     </row>
@@ -1529,14 +1454,10 @@
       <c r="J30" s="15">
         <v>307199</v>
       </c>
-      <c r="L30" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="M30" s="11"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="L30" s="35"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="35"/>
       <c r="R30" s="13"/>
       <c r="S30" s="14"/>
       <c r="T30" s="14"/>
@@ -1546,46 +1467,36 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="L31" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="M31" s="11"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L32" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="M32" s="13"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="R32" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="S32" s="34"/>
-      <c r="T32" s="34"/>
-      <c r="U32" s="34"/>
-      <c r="V32" s="34"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="35"/>
+      <c r="O31" s="35"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="35"/>
+      <c r="O32" s="35"/>
+      <c r="R32" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="S32" s="32"/>
+      <c r="T32" s="32"/>
+      <c r="U32" s="32"/>
+      <c r="V32" s="32"/>
     </row>
     <row r="33" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L33" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="O33" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="R33" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="S33" s="34"/>
-      <c r="T33" s="34"/>
-      <c r="U33" s="34"/>
-      <c r="V33" s="34"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="35"/>
+      <c r="R33" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="S33" s="32"/>
+      <c r="T33" s="32"/>
+      <c r="U33" s="32"/>
+      <c r="V33" s="32"/>
     </row>
     <row r="34" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
@@ -1601,17 +1512,15 @@
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
       <c r="J34" s="17"/>
-      <c r="L34" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="O34" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="R34" s="32"/>
-      <c r="S34" s="32"/>
-      <c r="T34" s="32"/>
-      <c r="U34" s="32"/>
-      <c r="V34" s="32"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="35"/>
+      <c r="R34" s="30"/>
+      <c r="S34" s="30"/>
+      <c r="T34" s="30"/>
+      <c r="U34" s="30"/>
+      <c r="V34" s="30"/>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
@@ -1631,17 +1540,15 @@
         <v>20</v>
       </c>
       <c r="J35" s="12"/>
-      <c r="L35" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="O35" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R35" s="32"/>
-      <c r="S35" s="32"/>
-      <c r="T35" s="32"/>
-      <c r="U35" s="32"/>
-      <c r="V35" s="32"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="35"/>
+      <c r="R35" s="30"/>
+      <c r="S35" s="30"/>
+      <c r="T35" s="30"/>
+      <c r="U35" s="30"/>
+      <c r="V35" s="30"/>
     </row>
     <row r="36" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
@@ -1659,36 +1566,32 @@
         <v>40</v>
       </c>
       <c r="J36" s="12"/>
-      <c r="L36" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="O36" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="R36" s="32"/>
-      <c r="S36" s="32"/>
-      <c r="T36" s="32"/>
-      <c r="U36" s="32"/>
-      <c r="V36" s="32"/>
+      <c r="L36" s="35"/>
+      <c r="M36" s="35"/>
+      <c r="N36" s="35"/>
+      <c r="O36" s="35"/>
+      <c r="R36" s="30"/>
+      <c r="S36" s="30"/>
+      <c r="T36" s="30"/>
+      <c r="U36" s="30"/>
+      <c r="V36" s="30"/>
     </row>
     <row r="37" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="E37" s="12"/>
       <c r="G37" s="11"/>
       <c r="J37" s="12"/>
-      <c r="L37" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="O37" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="R37" s="32"/>
-      <c r="S37" s="32"/>
-      <c r="T37" s="32"/>
-      <c r="U37" s="32"/>
-      <c r="V37" s="32"/>
-    </row>
-    <row r="38" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L37" s="35"/>
+      <c r="M37" s="35"/>
+      <c r="N37" s="35"/>
+      <c r="O37" s="35"/>
+      <c r="R37" s="30"/>
+      <c r="S37" s="30"/>
+      <c r="T37" s="30"/>
+      <c r="U37" s="30"/>
+      <c r="V37" s="30"/>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>5</v>
       </c>
@@ -1716,12 +1619,10 @@
       <c r="J38" s="18">
         <v>20</v>
       </c>
-      <c r="L38" s="13"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="15" t="s">
-        <v>14</v>
-      </c>
+      <c r="L38" s="35"/>
+      <c r="M38" s="35"/>
+      <c r="N38" s="35"/>
+      <c r="O38" s="35"/>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
@@ -1749,6 +1650,10 @@
       <c r="J39" s="12">
         <v>25</v>
       </c>
+      <c r="L39" s="35"/>
+      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="35"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>

</xml_diff>

<commit_message>
BILI - better version - show freezed pic
Signed-off-by: idowein <ido.weinstock@gmail.com>
</commit_message>
<xml_diff>
--- a/datasheets/bram2vga.xlsx
+++ b/datasheets/bram2vga.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idowe\Projects\Digital-Zoom-FPGA\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71444345-1000-4B83-8200-44C7E231B966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8855781E-DB29-40FE-ADDE-36FB9B41C56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9670E6A7-4A90-4DCF-AC2B-294B8B9A454C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
   <si>
     <t>BRAM</t>
   </si>
@@ -140,24 +140,12 @@
     <t>clkb - 25MHz</t>
   </si>
   <si>
-    <t xml:space="preserve">pix1 - 0 </t>
-  </si>
-  <si>
     <t>clka - 25 mhz</t>
   </si>
   <si>
     <t>clkb - 25 mhz</t>
   </si>
   <si>
-    <t>pix2 - 40 ns</t>
-  </si>
-  <si>
-    <t>pix3 - 80</t>
-  </si>
-  <si>
-    <t>pix4 - 120</t>
-  </si>
-  <si>
     <t>( 200 ns / 16 px ) = 12.5 ns -&gt; 80 mhz</t>
   </si>
   <si>
@@ -167,21 +155,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>output to small bili - 320</t>
-  </si>
-  <si>
-    <t>pix 6 &amp; output x 4 - 200</t>
-  </si>
-  <si>
-    <t>pix 5 &amp; output x 4 - 160</t>
-  </si>
-  <si>
-    <t>pix 7 &amp; output x 4 - 240</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pix 8 - 280 </t>
-  </si>
-  <si>
     <t>לחשב בלי אנסיינגד אלא עם דאון-טו</t>
   </si>
   <si>
@@ -243,6 +216,70 @@
   </si>
   <si>
     <t>pixel_in - 25 mhz (40 ns)</t>
+  </si>
+  <si>
+    <t>each 4 pixels (6.25 mhz) packet is filled</t>
+  </si>
+  <si>
+    <t>Nir's queries:</t>
+  </si>
+  <si>
+    <t>a.</t>
+  </si>
+  <si>
+    <t>should the interpolation pixels be calculated by signals / by variables?</t>
+  </si>
+  <si>
+    <t>b.</t>
+  </si>
+  <si>
+    <t>how much time would it take?</t>
+  </si>
+  <si>
+    <t>BILI_TOP:</t>
+  </si>
+  <si>
+    <t>pix1 - 40 ns</t>
+  </si>
+  <si>
+    <t>pix2 - 80 ns</t>
+  </si>
+  <si>
+    <t>pix3 - 120 ns</t>
+  </si>
+  <si>
+    <t>pix4 - 160 nS</t>
+  </si>
+  <si>
+    <t>c.</t>
+  </si>
+  <si>
+    <t>Should A, B, C, D be variable so they would be sampled immediately?</t>
+  </si>
+  <si>
+    <t>pix 5 &amp; output x 4 - 200</t>
+  </si>
+  <si>
+    <t>pix 6 &amp; output x 4 - 240</t>
+  </si>
+  <si>
+    <t>pix 7 &amp; output x 4 - 280</t>
+  </si>
+  <si>
+    <t>pix 8 - 320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A, B, C, D - 160 nS
+</t>
+  </si>
+  <si>
+    <t>calc - 200 nS</t>
+  </si>
+  <si>
+    <t>A, B, C, D - 280 nS</t>
+  </si>
+  <si>
+    <t>calc - 300 nS</t>
   </si>
 </sst>
 </file>
@@ -272,7 +309,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -336,6 +373,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -476,6 +519,14 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -812,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05C238A-0561-4BB7-9A92-291FE0D71310}">
-  <dimension ref="A1:V43"/>
+  <dimension ref="A1:X43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -828,12 +879,12 @@
     <col min="9" max="9" width="19.125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="13" width="23.25" customWidth="1"/>
-    <col min="16" max="16" width="30.375" customWidth="1"/>
-    <col min="17" max="17" width="11.25" customWidth="1"/>
+    <col min="12" max="15" width="23.25" customWidth="1"/>
+    <col min="18" max="18" width="30.375" customWidth="1"/>
+    <col min="19" max="19" width="11.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -844,22 +895,22 @@
         <v>6</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="M1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -888,25 +939,27 @@
       </c>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="5">
+      <c r="T2" s="5">
         <v>0</v>
       </c>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7">
+      <c r="U2" s="7"/>
+      <c r="V2" s="7">
         <v>0.6</v>
       </c>
-      <c r="U2" s="18">
+      <c r="W2" s="18">
         <v>1</v>
       </c>
-      <c r="V2" s="17"/>
-    </row>
-    <row r="3" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="X2" s="17"/>
+    </row>
+    <row r="3" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -929,26 +982,28 @@
         <v>639</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L3" s="27" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="M3" s="35"/>
       <c r="N3" s="35"/>
-      <c r="O3" s="12"/>
-      <c r="Q3" t="s">
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="12"/>
+      <c r="S3" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="11">
+      <c r="T3" s="11">
         <v>106.6</v>
       </c>
-      <c r="U3" s="12">
+      <c r="W3" s="12">
         <v>101</v>
       </c>
-      <c r="V3" s="12"/>
-    </row>
-    <row r="4" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="X3" s="12"/>
+    </row>
+    <row r="4" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>320</v>
       </c>
@@ -964,28 +1019,30 @@
       <c r="F4" s="11"/>
       <c r="J4" s="12"/>
       <c r="K4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="M4" s="35"/>
-      <c r="N4" s="35" t="s">
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="12"/>
-      <c r="Q4" t="s">
-        <v>41</v>
-      </c>
-      <c r="R4" s="11">
+      <c r="Q4" s="12"/>
+      <c r="S4" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="11">
         <v>210</v>
       </c>
-      <c r="U4" s="12">
+      <c r="W4" s="12">
         <v>202</v>
       </c>
-      <c r="V4" s="12"/>
-    </row>
-    <row r="5" spans="1:22" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X4" s="12"/>
+    </row>
+    <row r="5" spans="1:24" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>320</v>
       </c>
@@ -1001,122 +1058,132 @@
       <c r="F5" s="11"/>
       <c r="J5" s="12"/>
       <c r="L5" s="11" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="M5" s="35"/>
-      <c r="N5" s="35" t="s">
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="12"/>
-      <c r="P5" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="12"/>
+      <c r="R5" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" t="s">
         <v>27</v>
       </c>
-      <c r="R5" s="19">
+      <c r="T5" s="19">
         <v>320</v>
       </c>
-      <c r="S5" s="14">
+      <c r="U5" s="14">
         <v>320.3</v>
       </c>
-      <c r="T5" s="14">
+      <c r="V5" s="14">
         <v>320.60000000000002</v>
       </c>
-      <c r="U5" s="20">
+      <c r="W5" s="20">
         <v>321</v>
       </c>
-      <c r="V5" s="12"/>
-    </row>
-    <row r="6" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="X5" s="12"/>
+    </row>
+    <row r="6" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F6" s="11"/>
       <c r="J6" s="12"/>
       <c r="L6" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="M6" s="36"/>
-      <c r="N6" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="12"/>
-      <c r="Q6" t="s">
+      <c r="Q6" s="12"/>
+      <c r="S6" t="s">
         <v>28</v>
       </c>
-      <c r="R6" s="11"/>
-      <c r="V6" s="12"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="T6" s="11"/>
+      <c r="X6" s="12"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="F7" s="11"/>
       <c r="J7" s="12"/>
       <c r="L7" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="M7" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="N7" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="39"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="12"/>
-      <c r="Q7" t="s">
+      <c r="Q7" s="12"/>
+      <c r="S7" t="s">
         <v>29</v>
       </c>
-      <c r="R7" s="11"/>
-      <c r="V7" s="12"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="T7" s="11"/>
+      <c r="X7" s="12"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F8" s="11"/>
       <c r="J8" s="12"/>
       <c r="L8" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="M8" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="N8" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="12"/>
-      <c r="Q8" t="s">
+      <c r="Q8" s="12"/>
+      <c r="S8" t="s">
         <v>31</v>
       </c>
-      <c r="R8" s="11"/>
-      <c r="V8" s="12"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="T8" s="11"/>
+      <c r="X8" s="12"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="31"/>
       <c r="F9" s="11"/>
       <c r="J9" s="12"/>
       <c r="L9" s="11"/>
-      <c r="M9" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="N9" s="35" t="s">
+      <c r="M9" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="12"/>
-      <c r="Q9" t="s">
+      <c r="Q9" s="12"/>
+      <c r="S9" t="s">
         <v>33</v>
       </c>
-      <c r="R9" s="11"/>
-      <c r="V9" s="12"/>
-    </row>
-    <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="T9" s="11"/>
+      <c r="X9" s="12"/>
+    </row>
+    <row r="10" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C10" s="28"/>
       <c r="D10" s="28"/>
@@ -1130,36 +1197,38 @@
         <v>76799</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="M10" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="N10" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="M10" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10" s="35"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q10" t="s">
+      <c r="Q10" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="S10" t="s">
         <v>32</v>
       </c>
-      <c r="R10" s="13">
+      <c r="T10" s="13">
         <v>76480</v>
       </c>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
       <c r="U10" s="14"/>
-      <c r="V10" s="15">
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="15">
         <v>76799</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="31"/>
@@ -1169,36 +1238,44 @@
       <c r="I11" s="7"/>
       <c r="J11" s="17"/>
       <c r="L11" s="11"/>
-      <c r="M11" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="N11" s="35" t="s">
+      <c r="M11" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="N11" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="O11" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="P11" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="O11" s="12"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
+      <c r="Q11" s="12"/>
+      <c r="T11" s="16"/>
       <c r="U11" s="7"/>
-      <c r="V11" s="17"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="17"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="F12" s="11"/>
       <c r="J12" s="12"/>
       <c r="L12" s="11"/>
-      <c r="M12" s="35" t="s">
+      <c r="M12" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="N12" s="35"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q12" s="12"/>
+      <c r="T12" s="11"/>
+      <c r="X12" s="12"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>45</v>
-      </c>
-      <c r="N12" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="O12" s="12"/>
-      <c r="R12" s="11"/>
-      <c r="V12" s="12"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>54</v>
       </c>
       <c r="F13" s="11"/>
       <c r="H13">
@@ -1207,22 +1284,24 @@
       <c r="I13" s="28"/>
       <c r="J13" s="12"/>
       <c r="L13" s="11"/>
-      <c r="M13" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="N13" s="35" t="s">
+      <c r="M13" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="N13" s="35"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="O13" s="12"/>
-      <c r="R13" s="11"/>
-      <c r="V13" s="12"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Q13" s="12"/>
+      <c r="T13" s="11"/>
+      <c r="X13" s="12"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F14" s="11"/>
       <c r="H14">
@@ -1231,22 +1310,24 @@
       <c r="I14" s="28"/>
       <c r="J14" s="12"/>
       <c r="L14" s="11"/>
-      <c r="M14" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="N14" s="35" t="s">
+      <c r="M14" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="O14" s="12"/>
-      <c r="R14" s="11"/>
-      <c r="V14" s="12"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Q14" s="12"/>
+      <c r="T14" s="11"/>
+      <c r="X14" s="12"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F15" s="11"/>
       <c r="H15">
@@ -1255,19 +1336,23 @@
       <c r="I15" s="28"/>
       <c r="J15" s="12"/>
       <c r="L15" s="11"/>
-      <c r="M15" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="N15" s="35" t="s">
+      <c r="M15" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="N15" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="O15" s="36"/>
+      <c r="P15" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="12"/>
-      <c r="R15" s="11"/>
-      <c r="V15" s="12"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Q15" s="12"/>
+      <c r="T15" s="11"/>
+      <c r="X15" s="12"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F16" s="11"/>
       <c r="H16">
@@ -1276,35 +1361,38 @@
       <c r="I16" s="28"/>
       <c r="J16" s="12"/>
       <c r="L16" s="11"/>
-      <c r="M16" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="N16" s="35" t="s">
+      <c r="N16" s="35"/>
+      <c r="O16" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="P16" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="O16" s="12"/>
-      <c r="R16" s="11"/>
-      <c r="V16" s="12"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Q16" s="12"/>
+      <c r="T16" s="11"/>
+      <c r="X16" s="12"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F17" s="11"/>
       <c r="J17" s="12"/>
       <c r="L17" s="11"/>
       <c r="M17" s="35"/>
-      <c r="N17" s="35" t="s">
+      <c r="N17" s="35"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="O17" s="12"/>
-      <c r="R17" s="11"/>
-      <c r="V17" s="12"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Q17" s="12"/>
+      <c r="T17" s="11"/>
+      <c r="X17" s="12"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="F18" s="11"/>
       <c r="H18">
         <v>5</v>
@@ -1313,19 +1401,21 @@
       <c r="J18" s="12"/>
       <c r="L18" s="11"/>
       <c r="M18" s="35"/>
-      <c r="N18" s="35" t="s">
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="O18" s="12"/>
-      <c r="R18" s="11"/>
-      <c r="V18" s="12"/>
-    </row>
-    <row r="19" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q18" s="12"/>
+      <c r="T18" s="11"/>
+      <c r="X18" s="12"/>
+    </row>
+    <row r="19" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="F19" s="11"/>
       <c r="H19">
@@ -1335,24 +1425,29 @@
       <c r="J19" s="12"/>
       <c r="L19" s="13"/>
       <c r="M19" s="14"/>
-      <c r="N19" s="14" t="s">
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="O19" s="15"/>
-      <c r="R19" s="11"/>
-      <c r="V19" s="12"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Q19" s="15"/>
+      <c r="T19" s="11"/>
+      <c r="X19" s="12"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="F20" s="11"/>
       <c r="H20">
         <v>7</v>
       </c>
       <c r="I20" s="29"/>
       <c r="J20" s="12"/>
-      <c r="R20" s="11"/>
-      <c r="V20" s="12"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="T20" s="11"/>
+      <c r="X20" s="12"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
       <c r="F21" s="11"/>
       <c r="H21">
         <v>8</v>
@@ -1363,90 +1458,137 @@
       <c r="M21" s="35"/>
       <c r="N21" s="35"/>
       <c r="O21" s="35"/>
-      <c r="R21" s="11"/>
-      <c r="V21" s="12"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="T21" s="11"/>
+      <c r="X21" s="12"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="F22" s="11"/>
       <c r="J22" s="12"/>
       <c r="L22" s="36"/>
       <c r="M22" s="35"/>
       <c r="N22" s="35"/>
       <c r="O22" s="35"/>
-      <c r="R22" s="11"/>
-      <c r="V22" s="12"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P22" s="35"/>
+      <c r="Q22" s="35"/>
+      <c r="T22" s="11"/>
+      <c r="X22" s="12"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
+        <v>63</v>
+      </c>
       <c r="F23" s="11"/>
       <c r="J23" s="12"/>
       <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
+      <c r="M23" s="35" t="s">
+        <v>38</v>
+      </c>
       <c r="N23" s="35"/>
       <c r="O23" s="35"/>
-      <c r="R23" s="11"/>
-      <c r="V23" s="12"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P23" s="35"/>
+      <c r="Q23" s="35"/>
+      <c r="T23" s="11"/>
+      <c r="X23" s="12"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" t="s">
+        <v>65</v>
+      </c>
       <c r="F24" s="11"/>
       <c r="J24" s="12"/>
       <c r="L24" s="35"/>
       <c r="M24" s="35"/>
       <c r="N24" s="35"/>
       <c r="O24" s="35"/>
-      <c r="R24" s="11"/>
-      <c r="V24" s="12"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P24" s="35"/>
+      <c r="Q24" s="35"/>
+      <c r="T24" s="11"/>
+      <c r="X24" s="12"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s">
+        <v>72</v>
+      </c>
       <c r="F25" s="11"/>
       <c r="J25" s="12"/>
       <c r="L25" s="35"/>
       <c r="M25" s="36"/>
       <c r="N25" s="36"/>
-      <c r="O25" s="35"/>
-      <c r="R25" s="11"/>
-      <c r="V25" s="12"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="35"/>
+      <c r="T25" s="11"/>
+      <c r="X25" s="12"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="F26" s="11"/>
       <c r="J26" s="12"/>
       <c r="L26" s="35"/>
       <c r="M26" s="35"/>
       <c r="N26" s="35"/>
       <c r="O26" s="35"/>
-      <c r="R26" s="11"/>
-      <c r="V26" s="12"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P26" s="35"/>
+      <c r="Q26" s="35"/>
+      <c r="T26" s="11"/>
+      <c r="X26" s="12"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="F27" s="11"/>
       <c r="J27" s="12"/>
       <c r="L27" s="35"/>
       <c r="M27" s="35"/>
       <c r="N27" s="35"/>
       <c r="O27" s="35"/>
-      <c r="R27" s="11"/>
-      <c r="V27" s="12"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P27" s="35"/>
+      <c r="Q27" s="35"/>
+      <c r="T27" s="11"/>
+      <c r="X27" s="12"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="F28" s="11"/>
       <c r="J28" s="12"/>
       <c r="L28" s="36"/>
       <c r="M28" s="35"/>
       <c r="N28" s="35"/>
       <c r="O28" s="35"/>
-      <c r="R28" s="11"/>
-      <c r="V28" s="12"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P28" s="35"/>
+      <c r="Q28" s="35"/>
+      <c r="T28" s="11"/>
+      <c r="X28" s="12"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="F29" s="11"/>
       <c r="J29" s="12"/>
       <c r="L29" s="35"/>
       <c r="M29" s="35"/>
       <c r="N29" s="35"/>
       <c r="O29" s="35"/>
-      <c r="R29" s="11"/>
-      <c r="V29" s="12"/>
-    </row>
-    <row r="30" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P29" s="35"/>
+      <c r="Q29" s="35"/>
+      <c r="T29" s="11"/>
+      <c r="X29" s="12"/>
+    </row>
+    <row r="30" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F30" s="13"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -1458,47 +1600,55 @@
       <c r="M30" s="35"/>
       <c r="N30" s="35"/>
       <c r="O30" s="35"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="14"/>
-      <c r="T30" s="14"/>
+      <c r="P30" s="35"/>
+      <c r="Q30" s="35"/>
+      <c r="T30" s="13"/>
       <c r="U30" s="14"/>
-      <c r="V30" s="15">
+      <c r="V30" s="14"/>
+      <c r="W30" s="14"/>
+      <c r="X30" s="15">
         <v>307199</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="L31" s="35"/>
       <c r="M31" s="35"/>
       <c r="N31" s="35"/>
       <c r="O31" s="35"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P31" s="35"/>
+      <c r="Q31" s="35"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="L32" s="35"/>
       <c r="M32" s="35"/>
       <c r="N32" s="35"/>
       <c r="O32" s="35"/>
-      <c r="R32" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="S32" s="32"/>
-      <c r="T32" s="32"/>
+      <c r="P32" s="35"/>
+      <c r="Q32" s="35"/>
+      <c r="T32" s="32" t="s">
+        <v>39</v>
+      </c>
       <c r="U32" s="32"/>
       <c r="V32" s="32"/>
-    </row>
-    <row r="33" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="W32" s="32"/>
+      <c r="X32" s="32"/>
+    </row>
+    <row r="33" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L33" s="35"/>
       <c r="M33" s="35"/>
       <c r="N33" s="35"/>
       <c r="O33" s="35"/>
-      <c r="R33" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="S33" s="32"/>
-      <c r="T33" s="32"/>
+      <c r="P33" s="35"/>
+      <c r="Q33" s="35"/>
+      <c r="T33" s="32" t="s">
+        <v>40</v>
+      </c>
       <c r="U33" s="32"/>
       <c r="V33" s="32"/>
-    </row>
-    <row r="34" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="W33" s="32"/>
+      <c r="X33" s="32"/>
+    </row>
+    <row r="34" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>3</v>
       </c>
@@ -1516,13 +1666,15 @@
       <c r="M34" s="35"/>
       <c r="N34" s="35"/>
       <c r="O34" s="35"/>
-      <c r="R34" s="30"/>
-      <c r="S34" s="30"/>
+      <c r="P34" s="35"/>
+      <c r="Q34" s="35"/>
       <c r="T34" s="30"/>
       <c r="U34" s="30"/>
       <c r="V34" s="30"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W34" s="30"/>
+      <c r="X34" s="30"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>0</v>
       </c>
@@ -1544,13 +1696,15 @@
       <c r="M35" s="35"/>
       <c r="N35" s="35"/>
       <c r="O35" s="35"/>
-      <c r="R35" s="30"/>
-      <c r="S35" s="30"/>
+      <c r="P35" s="35"/>
+      <c r="Q35" s="35"/>
       <c r="T35" s="30"/>
       <c r="U35" s="30"/>
       <c r="V35" s="30"/>
-    </row>
-    <row r="36" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="W35" s="30"/>
+      <c r="X35" s="30"/>
+    </row>
+    <row r="36" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="19">
         <v>30</v>
@@ -1570,13 +1724,15 @@
       <c r="M36" s="35"/>
       <c r="N36" s="35"/>
       <c r="O36" s="35"/>
-      <c r="R36" s="30"/>
-      <c r="S36" s="30"/>
+      <c r="P36" s="35"/>
+      <c r="Q36" s="35"/>
       <c r="T36" s="30"/>
       <c r="U36" s="30"/>
       <c r="V36" s="30"/>
-    </row>
-    <row r="37" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="W36" s="30"/>
+      <c r="X36" s="30"/>
+    </row>
+    <row r="37" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="E37" s="12"/>
       <c r="G37" s="11"/>
@@ -1585,13 +1741,15 @@
       <c r="M37" s="35"/>
       <c r="N37" s="35"/>
       <c r="O37" s="35"/>
-      <c r="R37" s="30"/>
-      <c r="S37" s="30"/>
+      <c r="P37" s="35"/>
+      <c r="Q37" s="35"/>
       <c r="T37" s="30"/>
       <c r="U37" s="30"/>
       <c r="V37" s="30"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W37" s="30"/>
+      <c r="X37" s="30"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>5</v>
       </c>
@@ -1623,8 +1781,10 @@
       <c r="M38" s="35"/>
       <c r="N38" s="35"/>
       <c r="O38" s="35"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P38" s="35"/>
+      <c r="Q38" s="35"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
       <c r="B39" s="22">
         <v>10</v>
@@ -1654,8 +1814,10 @@
       <c r="M39" s="35"/>
       <c r="N39" s="35"/>
       <c r="O39" s="35"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P39" s="35"/>
+      <c r="Q39" s="35"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
       <c r="B40" s="9">
         <v>30</v>
@@ -1682,7 +1844,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="19">
         <v>30</v>
@@ -1709,8 +1871,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="G43" s="18">
         <v>20</v>
       </c>
@@ -1723,9 +1885,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="R32:V32"/>
-    <mergeCell ref="R33:V33"/>
+  <mergeCells count="3">
+    <mergeCell ref="T32:X32"/>
+    <mergeCell ref="T33:X33"/>
+    <mergeCell ref="M6:M7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
project presentation - v0.3
Signed-off-by: Dvir Hershkovits <dvirhersh@gmail.com>
</commit_message>
<xml_diff>
--- a/datasheets/bram2vga.xlsx
+++ b/datasheets/bram2vga.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idowe\Projects\Digital-Zoom-FPGA\datasheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital-Zoom-FPGA\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8855781E-DB29-40FE-ADDE-36FB9B41C56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6496D960-C3F6-4664-B16F-09564AF60033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9670E6A7-4A90-4DCF-AC2B-294B8B9A454C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9670E6A7-4A90-4DCF-AC2B-294B8B9A454C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -290,13 +290,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -304,7 +304,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -475,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -512,23 +512,19 @@
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,25 +859,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05C238A-0561-4BB7-9A92-291FE0D71310}">
-  <dimension ref="A1:X43"/>
+  <dimension ref="A1:X77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.375" customWidth="1"/>
-    <col min="4" max="4" width="47.625" customWidth="1"/>
+    <col min="1" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="15" width="23.25" customWidth="1"/>
-    <col min="18" max="18" width="30.375" customWidth="1"/>
-    <col min="19" max="19" width="11.25" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="23.28515625" customWidth="1"/>
+    <col min="18" max="18" width="30.42578125" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -891,16 +886,16 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="33" t="s">
         <v>53</v>
       </c>
       <c r="M1" t="s">
@@ -910,7 +905,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -959,7 +954,7 @@
       </c>
       <c r="X2" s="17"/>
     </row>
-    <row r="3" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -987,10 +982,6 @@
       <c r="L3" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
       <c r="Q3" s="12"/>
       <c r="S3" t="s">
         <v>30</v>
@@ -1003,7 +994,7 @@
       </c>
       <c r="X3" s="12"/>
     </row>
-    <row r="4" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>320</v>
       </c>
@@ -1024,10 +1015,7 @@
       <c r="L4" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35" t="s">
+      <c r="P4" t="s">
         <v>9</v>
       </c>
       <c r="Q4" s="12"/>
@@ -1042,7 +1030,7 @@
       </c>
       <c r="X4" s="12"/>
     </row>
-    <row r="5" spans="1:24" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>320</v>
       </c>
@@ -1060,10 +1048,7 @@
       <c r="L5" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35" t="s">
+      <c r="P5" t="s">
         <v>10</v>
       </c>
       <c r="Q5" s="12"/>
@@ -1087,18 +1072,18 @@
       </c>
       <c r="X5" s="12"/>
     </row>
-    <row r="6" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F6" s="11"/>
       <c r="J6" s="12"/>
       <c r="L6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="39" t="s">
+      <c r="M6" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="35" t="s">
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" t="s">
         <v>11</v>
       </c>
       <c r="Q6" s="12"/>
@@ -1108,16 +1093,14 @@
       <c r="T6" s="11"/>
       <c r="X6" s="12"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F7" s="11"/>
       <c r="J7" s="12"/>
       <c r="L7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="M7" s="39"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35" t="s">
+      <c r="M7" s="37"/>
+      <c r="P7" t="s">
         <v>12</v>
       </c>
       <c r="Q7" s="12"/>
@@ -1127,7 +1110,7 @@
       <c r="T7" s="11"/>
       <c r="X7" s="12"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -1136,12 +1119,10 @@
       <c r="L8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="M8" s="37" t="s">
+      <c r="M8" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="35" t="s">
+      <c r="P8" t="s">
         <v>15</v>
       </c>
       <c r="Q8" s="12"/>
@@ -1151,7 +1132,7 @@
       <c r="T8" s="11"/>
       <c r="X8" s="12"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1163,12 +1144,10 @@
       <c r="F9" s="11"/>
       <c r="J9" s="12"/>
       <c r="L9" s="11"/>
-      <c r="M9" s="37" t="s">
+      <c r="M9" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="N9" s="35"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35" t="s">
+      <c r="P9" t="s">
         <v>18</v>
       </c>
       <c r="Q9" s="12"/>
@@ -1178,7 +1157,7 @@
       <c r="T9" s="11"/>
       <c r="X9" s="12"/>
     </row>
-    <row r="10" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1199,12 +1178,10 @@
       <c r="L10" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="M10" s="37" t="s">
+      <c r="M10" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35" t="s">
+      <c r="P10" t="s">
         <v>19</v>
       </c>
       <c r="Q10" s="12" t="s">
@@ -1223,7 +1200,7 @@
         <v>76799</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1238,16 +1215,16 @@
       <c r="I11" s="7"/>
       <c r="J11" s="17"/>
       <c r="L11" s="11"/>
-      <c r="M11" s="37" t="s">
+      <c r="M11" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="N11" s="36" t="s">
+      <c r="N11" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="O11" s="36" t="s">
+      <c r="O11" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="P11" s="35" t="s">
+      <c r="P11" t="s">
         <v>20</v>
       </c>
       <c r="Q11" s="12"/>
@@ -1257,23 +1234,21 @@
       <c r="W11" s="7"/>
       <c r="X11" s="17"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F12" s="11"/>
       <c r="J12" s="12"/>
       <c r="L12" s="11"/>
-      <c r="M12" s="38" t="s">
+      <c r="M12" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35" t="s">
+      <c r="P12" t="s">
         <v>16</v>
       </c>
       <c r="Q12" s="12"/>
       <c r="T12" s="11"/>
       <c r="X12" s="12"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1284,19 +1259,17 @@
       <c r="I13" s="28"/>
       <c r="J13" s="12"/>
       <c r="L13" s="11"/>
-      <c r="M13" s="38" t="s">
+      <c r="M13" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35" t="s">
+      <c r="P13" t="s">
         <v>21</v>
       </c>
       <c r="Q13" s="12"/>
       <c r="T13" s="11"/>
       <c r="X13" s="12"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1310,19 +1283,17 @@
       <c r="I14" s="28"/>
       <c r="J14" s="12"/>
       <c r="L14" s="11"/>
-      <c r="M14" s="38" t="s">
+      <c r="M14" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35" t="s">
+      <c r="P14" t="s">
         <v>22</v>
       </c>
       <c r="Q14" s="12"/>
       <c r="T14" s="11"/>
       <c r="X14" s="12"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1336,21 +1307,21 @@
       <c r="I15" s="28"/>
       <c r="J15" s="12"/>
       <c r="L15" s="11"/>
-      <c r="M15" s="38" t="s">
+      <c r="M15" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="N15" s="36" t="s">
+      <c r="N15" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="O15" s="36"/>
-      <c r="P15" s="35" t="s">
+      <c r="O15" s="34"/>
+      <c r="P15" t="s">
         <v>23</v>
       </c>
       <c r="Q15" s="12"/>
       <c r="T15" s="11"/>
       <c r="X15" s="12"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>48</v>
       </c>
@@ -1361,18 +1332,17 @@
       <c r="I16" s="28"/>
       <c r="J16" s="12"/>
       <c r="L16" s="11"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35" t="s">
+      <c r="O16" t="s">
         <v>80</v>
       </c>
-      <c r="P16" s="35" t="s">
+      <c r="P16" t="s">
         <v>24</v>
       </c>
       <c r="Q16" s="12"/>
       <c r="T16" s="11"/>
       <c r="X16" s="12"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1382,17 +1352,14 @@
       <c r="F17" s="11"/>
       <c r="J17" s="12"/>
       <c r="L17" s="11"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35" t="s">
+      <c r="P17" t="s">
         <v>25</v>
       </c>
       <c r="Q17" s="12"/>
       <c r="T17" s="11"/>
       <c r="X17" s="12"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F18" s="11"/>
       <c r="H18">
         <v>5</v>
@@ -1400,17 +1367,14 @@
       <c r="I18" s="29"/>
       <c r="J18" s="12"/>
       <c r="L18" s="11"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35" t="s">
+      <c r="P18" t="s">
         <v>17</v>
       </c>
       <c r="Q18" s="12"/>
       <c r="T18" s="11"/>
       <c r="X18" s="12"/>
     </row>
-    <row r="19" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -1434,7 +1398,7 @@
       <c r="T19" s="11"/>
       <c r="X19" s="12"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F20" s="11"/>
       <c r="H20">
         <v>7</v>
@@ -1444,7 +1408,7 @@
       <c r="T20" s="11"/>
       <c r="X20" s="12"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -1454,34 +1418,23 @@
       </c>
       <c r="I21" s="29"/>
       <c r="J21" s="12"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="35"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="35"/>
       <c r="T21" s="11"/>
       <c r="X21" s="12"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="34" t="s">
         <v>66</v>
       </c>
       <c r="F22" s="11"/>
       <c r="J22" s="12"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="35"/>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
+      <c r="L22" s="34"/>
       <c r="T22" s="11"/>
       <c r="X22" s="12"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>62</v>
       </c>
@@ -1490,18 +1443,13 @@
       </c>
       <c r="F23" s="11"/>
       <c r="J23" s="12"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35" t="s">
+      <c r="M23" t="s">
         <v>38</v>
       </c>
-      <c r="N23" s="35"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="35"/>
-      <c r="Q23" s="35"/>
       <c r="T23" s="11"/>
       <c r="X23" s="12"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>64</v>
       </c>
@@ -1510,16 +1458,10 @@
       </c>
       <c r="F24" s="11"/>
       <c r="J24" s="12"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="35"/>
-      <c r="P24" s="35"/>
-      <c r="Q24" s="35"/>
       <c r="T24" s="11"/>
       <c r="X24" s="12"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>2</v>
       </c>
@@ -1531,64 +1473,39 @@
       </c>
       <c r="F25" s="11"/>
       <c r="J25" s="12"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="36"/>
-      <c r="O25" s="36"/>
-      <c r="P25" s="36"/>
-      <c r="Q25" s="35"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
+      <c r="P25" s="34"/>
       <c r="T25" s="11"/>
       <c r="X25" s="12"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F26" s="11"/>
       <c r="J26" s="12"/>
-      <c r="L26" s="35"/>
-      <c r="M26" s="35"/>
-      <c r="N26" s="35"/>
-      <c r="O26" s="35"/>
-      <c r="P26" s="35"/>
-      <c r="Q26" s="35"/>
       <c r="T26" s="11"/>
       <c r="X26" s="12"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F27" s="11"/>
       <c r="J27" s="12"/>
-      <c r="L27" s="35"/>
-      <c r="M27" s="35"/>
-      <c r="N27" s="35"/>
-      <c r="O27" s="35"/>
-      <c r="P27" s="35"/>
-      <c r="Q27" s="35"/>
       <c r="T27" s="11"/>
       <c r="X27" s="12"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F28" s="11"/>
       <c r="J28" s="12"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="35"/>
-      <c r="N28" s="35"/>
-      <c r="O28" s="35"/>
-      <c r="P28" s="35"/>
-      <c r="Q28" s="35"/>
+      <c r="L28" s="34"/>
       <c r="T28" s="11"/>
       <c r="X28" s="12"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F29" s="11"/>
       <c r="J29" s="12"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="35"/>
-      <c r="N29" s="35"/>
-      <c r="O29" s="35"/>
-      <c r="P29" s="35"/>
-      <c r="Q29" s="35"/>
       <c r="T29" s="11"/>
       <c r="X29" s="12"/>
     </row>
-    <row r="30" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F30" s="13"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -1596,12 +1513,6 @@
       <c r="J30" s="15">
         <v>307199</v>
       </c>
-      <c r="L30" s="35"/>
-      <c r="M30" s="35"/>
-      <c r="N30" s="35"/>
-      <c r="O30" s="35"/>
-      <c r="P30" s="35"/>
-      <c r="Q30" s="35"/>
       <c r="T30" s="13"/>
       <c r="U30" s="14"/>
       <c r="V30" s="14"/>
@@ -1610,45 +1521,25 @@
         <v>307199</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="L31" s="35"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="35"/>
-      <c r="O31" s="35"/>
-      <c r="P31" s="35"/>
-      <c r="Q31" s="35"/>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="L32" s="35"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="35"/>
-      <c r="P32" s="35"/>
-      <c r="Q32" s="35"/>
-      <c r="T32" s="32" t="s">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="T32" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="U32" s="32"/>
-      <c r="V32" s="32"/>
-      <c r="W32" s="32"/>
-      <c r="X32" s="32"/>
-    </row>
-    <row r="33" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L33" s="35"/>
-      <c r="M33" s="35"/>
-      <c r="N33" s="35"/>
-      <c r="O33" s="35"/>
-      <c r="P33" s="35"/>
-      <c r="Q33" s="35"/>
-      <c r="T33" s="32" t="s">
+      <c r="U32" s="36"/>
+      <c r="V32" s="36"/>
+      <c r="W32" s="36"/>
+      <c r="X32" s="36"/>
+    </row>
+    <row r="33" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T33" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="U33" s="32"/>
-      <c r="V33" s="32"/>
-      <c r="W33" s="32"/>
-      <c r="X33" s="32"/>
-    </row>
-    <row r="34" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U33" s="36"/>
+      <c r="V33" s="36"/>
+      <c r="W33" s="36"/>
+      <c r="X33" s="36"/>
+    </row>
+    <row r="34" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
         <v>3</v>
       </c>
@@ -1662,19 +1553,13 @@
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
       <c r="J34" s="17"/>
-      <c r="L34" s="35"/>
-      <c r="M34" s="35"/>
-      <c r="N34" s="35"/>
-      <c r="O34" s="35"/>
-      <c r="P34" s="35"/>
-      <c r="Q34" s="35"/>
       <c r="T34" s="30"/>
       <c r="U34" s="30"/>
       <c r="V34" s="30"/>
       <c r="W34" s="30"/>
       <c r="X34" s="30"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>0</v>
       </c>
@@ -1692,19 +1577,13 @@
         <v>20</v>
       </c>
       <c r="J35" s="12"/>
-      <c r="L35" s="35"/>
-      <c r="M35" s="35"/>
-      <c r="N35" s="35"/>
-      <c r="O35" s="35"/>
-      <c r="P35" s="35"/>
-      <c r="Q35" s="35"/>
       <c r="T35" s="30"/>
       <c r="U35" s="30"/>
       <c r="V35" s="30"/>
       <c r="W35" s="30"/>
       <c r="X35" s="30"/>
     </row>
-    <row r="36" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
       <c r="B36" s="19">
         <v>30</v>
@@ -1720,36 +1599,24 @@
         <v>40</v>
       </c>
       <c r="J36" s="12"/>
-      <c r="L36" s="35"/>
-      <c r="M36" s="35"/>
-      <c r="N36" s="35"/>
-      <c r="O36" s="35"/>
-      <c r="P36" s="35"/>
-      <c r="Q36" s="35"/>
       <c r="T36" s="30"/>
       <c r="U36" s="30"/>
       <c r="V36" s="30"/>
       <c r="W36" s="30"/>
       <c r="X36" s="30"/>
     </row>
-    <row r="37" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11"/>
       <c r="E37" s="12"/>
       <c r="G37" s="11"/>
       <c r="J37" s="12"/>
-      <c r="L37" s="35"/>
-      <c r="M37" s="35"/>
-      <c r="N37" s="35"/>
-      <c r="O37" s="35"/>
-      <c r="P37" s="35"/>
-      <c r="Q37" s="35"/>
       <c r="T37" s="30"/>
       <c r="U37" s="30"/>
       <c r="V37" s="30"/>
       <c r="W37" s="30"/>
       <c r="X37" s="30"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>5</v>
       </c>
@@ -1777,14 +1644,8 @@
       <c r="J38" s="18">
         <v>20</v>
       </c>
-      <c r="L38" s="35"/>
-      <c r="M38" s="35"/>
-      <c r="N38" s="35"/>
-      <c r="O38" s="35"/>
-      <c r="P38" s="35"/>
-      <c r="Q38" s="35"/>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="22">
         <v>10</v>
@@ -1810,14 +1671,8 @@
       <c r="J39" s="12">
         <v>25</v>
       </c>
-      <c r="L39" s="35"/>
-      <c r="M39" s="35"/>
-      <c r="N39" s="35"/>
-      <c r="O39" s="35"/>
-      <c r="P39" s="35"/>
-      <c r="Q39" s="35"/>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="9">
         <v>30</v>
@@ -1844,7 +1699,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
       <c r="B41" s="19">
         <v>30</v>
@@ -1871,8 +1726,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G43" s="18">
         <v>20</v>
       </c>
@@ -1882,6 +1737,220 @@
       </c>
       <c r="J43" s="5">
         <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>0</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1</v>
+      </c>
+      <c r="G49" s="5">
+        <v>0</v>
+      </c>
+      <c r="H49" s="6">
+        <v>1</v>
+      </c>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="8">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1</v>
+      </c>
+      <c r="D50" s="2">
+        <v>1</v>
+      </c>
+      <c r="G50" s="9">
+        <v>320</v>
+      </c>
+      <c r="H50" s="4">
+        <v>321</v>
+      </c>
+      <c r="K50" s="10">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>320</v>
+      </c>
+      <c r="B51" s="3">
+        <v>320</v>
+      </c>
+      <c r="C51" s="4">
+        <v>321</v>
+      </c>
+      <c r="D51" s="4">
+        <v>321</v>
+      </c>
+      <c r="G51" s="11"/>
+      <c r="K51" s="12"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>320</v>
+      </c>
+      <c r="B52" s="3">
+        <v>320</v>
+      </c>
+      <c r="C52" s="4">
+        <v>321</v>
+      </c>
+      <c r="D52" s="4">
+        <v>321</v>
+      </c>
+      <c r="G52" s="11"/>
+      <c r="K52" s="12"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G53" s="11"/>
+      <c r="K53" s="12"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G54" s="11"/>
+      <c r="K54" s="12"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G55" s="11"/>
+      <c r="K55" s="12"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G56" s="11"/>
+      <c r="K56" s="12"/>
+    </row>
+    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G57" s="13">
+        <v>76480</v>
+      </c>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="15">
+        <v>76799</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G58" s="16"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="17"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G59" s="11"/>
+      <c r="K59" s="12"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G60" s="11"/>
+      <c r="I60" s="38"/>
+      <c r="J60" s="38"/>
+      <c r="K60" s="12"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G61" s="11"/>
+      <c r="I61" s="38"/>
+      <c r="J61" s="38"/>
+      <c r="K61" s="12"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G62" s="11"/>
+      <c r="I62" s="38"/>
+      <c r="J62" s="38"/>
+      <c r="K62" s="12"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G63" s="11"/>
+      <c r="I63" s="38"/>
+      <c r="J63" s="38"/>
+      <c r="K63" s="12"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G64" s="11"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="38"/>
+      <c r="K64" s="12"/>
+    </row>
+    <row r="65" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G65" s="11"/>
+      <c r="I65" s="38"/>
+      <c r="J65" s="38"/>
+      <c r="K65" s="12"/>
+    </row>
+    <row r="66" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G66" s="11"/>
+      <c r="I66" s="38"/>
+      <c r="J66" s="38"/>
+      <c r="K66" s="12"/>
+    </row>
+    <row r="67" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G67" s="11"/>
+      <c r="I67" s="38"/>
+      <c r="J67" s="38"/>
+      <c r="K67" s="12"/>
+    </row>
+    <row r="68" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G68" s="11"/>
+      <c r="I68" s="38"/>
+      <c r="J68" s="38"/>
+      <c r="K68" s="12"/>
+    </row>
+    <row r="69" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G69" s="11"/>
+      <c r="K69" s="12"/>
+    </row>
+    <row r="70" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G70" s="11"/>
+      <c r="K70" s="12"/>
+    </row>
+    <row r="71" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G71" s="11"/>
+      <c r="K71" s="12"/>
+    </row>
+    <row r="72" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G72" s="11"/>
+      <c r="K72" s="12"/>
+    </row>
+    <row r="73" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G73" s="11"/>
+      <c r="K73" s="12"/>
+    </row>
+    <row r="74" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G74" s="11"/>
+      <c r="K74" s="12"/>
+    </row>
+    <row r="75" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G75" s="11"/>
+      <c r="K75" s="12"/>
+    </row>
+    <row r="76" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G76" s="11"/>
+      <c r="K76" s="12"/>
+    </row>
+    <row r="77" spans="7:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G77" s="13"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="14"/>
+      <c r="K77" s="15">
+        <v>307199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>